<commit_message>
edit erb, convert csv xlsx
</commit_message>
<xml_diff>
--- a/crawler/publics/data.xlsx
+++ b/crawler/publics/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId4"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -73,12 +73,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="27.28988764044944"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="21.789887640449443"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.389887640449437"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.18988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="60.28988764044945"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="59.18988764044944"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -116,950 +116,950 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Mason Lane</t>
+          <t>Petra Goff</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>1-435-126-8820</t>
+          <t>1-367-480-1708</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>consectetuer.cursus@google.org</t>
+          <t>dictum.sapien.aenean@icloud.com</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Rogaland</t>
+          <t>Agder</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>Donec fringilla. Donec feugiat metus sit amet ante. Vivamus non</t>
+          <t>ultrices, mauris ipsum porta elit, a feugiat tellus lorem eu</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Cheryl Barry</t>
+          <t>Alyssa Chandler</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>1-126-615-5520</t>
+          <t>1-615-771-1021</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>ullamcorper.velit.in@hotmail.net</t>
+          <t>arcu.vestibulum@aol.couk</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>Tolima</t>
+          <t>Samsun</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>eu arcu. Morbi sit amet massa. Quisque porttitor eros nec</t>
+          <t>metus urna convallis erat, eget tincidunt dui augue eu tellus.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>Lacota Williams</t>
+          <t>Adara Whitley</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>1-514-347-7717</t>
+          <t>1-581-630-8134</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>ullamcorper.duis@protonmail.ca</t>
+          <t>mauris.blandit.mattis@yahoo.couk</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>North Jeolla</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>neque non quam. Pellentesque habitant morbi tristique senectus et netus</t>
+          <t>in consequat enim diam vel arcu. Curabitur ut odio vel</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>Jordan Donaldson</t>
+          <t>Aaron Thornton</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>1-312-813-5532</t>
+          <t>(116) 880-4806</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>sapien.gravida@hotmail.com</t>
+          <t>nullam.feugiat@yahoo.com</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>Alajuela</t>
+          <t>Kerala</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>dictum augue malesuada malesuada. Integer id magna et ipsum cursus</t>
+          <t>pede et risus. Quisque libero lacus, varius et, euismod et,</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>Lawrence Dunn</t>
+          <t>Camille Logan</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>(723) 267-6532</t>
+          <t>1-318-951-6726</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>nonummy.ultricies@hotmail.org</t>
+          <t>id.enim.curabitur@protonmail.ca</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>Zhōngnán</t>
+          <t>Benue</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>aliquam, enim nec tempus scelerisque, lorem ipsum sodales purus, in</t>
+          <t>metus. In lorem. Donec elementum, lorem ut aliquam iaculis, lacus</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>Keiko Adams</t>
+          <t>Kadeem Chang</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>1-467-533-7291</t>
+          <t>1-247-380-5998</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>magna.tellus@aol.net</t>
+          <t>dolor@outlook.ca</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>Luhansk oblast</t>
+          <t>Córdoba</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>ac, feugiat non, lobortis quis, pede. Suspendisse dui. Fusce diam</t>
+          <t>sapien, gravida non, sollicitudin a, malesuada id, erat. Etiam vestibulum</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>Travis Leonard</t>
+          <t>Brittany Manning</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>(529) 134-4610</t>
+          <t>1-821-239-5556</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>nulla.at@icloud.ca</t>
+          <t>ad.litora@aol.edu</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>KwaZulu-Natal</t>
+          <t>Warwickshire</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>ridiculus mus. Proin vel arcu eu odio tristique pharetra. Quisque</t>
+          <t>fringilla. Donec feugiat metus sit amet ante. Vivamus non lorem</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>Kibo Trevino</t>
+          <t>Nina English</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>1-825-745-4761</t>
+          <t>1-995-947-4451</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>fusce.feugiat.lorem@hotmail.org</t>
+          <t>interdum.libero@protonmail.net</t>
         </is>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Puno</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>lacus. Mauris non dui nec urna suscipit nonummy. Fusce fermentum</t>
+          <t>sapien. Nunc pulvinar arcu et pede. Nunc sed orci lobortis</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>Michael Fischer</t>
+          <t>Jena Delaney</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>(882) 364-9398</t>
+          <t>(236) 831-7636</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>a.magna@outlook.com</t>
+          <t>cum.sociis@hotmail.net</t>
         </is>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>Lubuskie</t>
+          <t>Bangsamoro</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>sed, est. Nunc laoreet lectus quis massa. Mauris vestibulum, neque</t>
+          <t>magna. Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Etiam</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>Nora Burke</t>
+          <t>Inez Trevino</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>1-736-674-8181</t>
+          <t>(327) 137-3307</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>quis.lectus@google.com</t>
+          <t>sed@google.net</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>Wielkopolskie</t>
+          <t>South Island</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>Mauris nulla. Integer urna. Vivamus molestie dapibus ligula. Aliquam erat</t>
+          <t>Integer id magna et ipsum cursus vestibulum. Mauris magna. Duis</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>Colby Frost</t>
+          <t>Hayfa Hampton</t>
         </is>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>(175) 513-3728</t>
+          <t>(761) 823-3825</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>cum.sociis@icloud.ca</t>
+          <t>convallis@hotmail.couk</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>Cesar</t>
+          <t>Haute-Normandie</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>nisi. Mauris nulla. Integer urna. Vivamus molestie dapibus ligula. Aliquam</t>
+          <t>tincidunt adipiscing. Mauris molestie pharetra nibh. Aliquam ornare, libero at</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>Kellie Cook</t>
+          <t>Dai Kirby</t>
         </is>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>1-534-764-6112</t>
+          <t>(617) 839-7545</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
         <is>
-          <t>faucibus.lectus@aol.edu</t>
+          <t>erat.neque@hotmail.edu</t>
         </is>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>Bolívar</t>
+          <t>North Island</t>
         </is>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>urna justo faucibus lectus, a sollicitudin orci sem eget massa.</t>
+          <t>lectus rutrum urna, nec luctus felis purus ac tellus. Suspendisse</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>Martin Mcintosh</t>
+          <t>Thane Hamilton</t>
         </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>(552) 886-7974</t>
+          <t>(651) 155-5139</t>
         </is>
       </c>
       <c r="C14" s="0" t="inlineStr">
         <is>
-          <t>vivamus@google.ca</t>
+          <t>eu.eros.nam@hotmail.ca</t>
         </is>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>Gangwon</t>
+          <t>New South Wales</t>
         </is>
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>Quisque ornare tortor at risus. Nunc ac sem ut dolor</t>
+          <t>at pretium aliquet, metus urna convallis erat, eget tincidunt dui</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>Tallulah Walton</t>
+          <t>Reuben Mccoy</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>(545) 297-5570</t>
+          <t>(826) 586-9725</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>sed.congue@google.org</t>
+          <t>praesent@aol.com</t>
         </is>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>Brussels Hoofdstedelijk Gewest</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>luctus lobortis. Class aptent taciti sociosqu ad litora torquent per</t>
+          <t>non dui nec urna suscipit nonummy. Fusce fermentum fermentum arcu.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>Cade Coleman</t>
+          <t>Gregory Pickett</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>(223) 758-1371</t>
+          <t>(938) 675-4511</t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
         <is>
-          <t>phasellus.fermentum@hotmail.org</t>
+          <t>eu.enim@yahoo.com</t>
         </is>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>Zhōngnán</t>
+          <t>Rivers</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>non dui nec urna suscipit nonummy. Fusce fermentum fermentum arcu.</t>
+          <t>sagittis augue, eu tempor erat neque non quam. Pellentesque habitant</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>Latifah Hubbard</t>
+          <t>Kyla Horn</t>
         </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>(657) 876-3751</t>
+          <t>1-644-356-8496</t>
         </is>
       </c>
       <c r="C17" s="0" t="inlineStr">
         <is>
-          <t>tempus.scelerisque.lorem@outlook.org</t>
+          <t>lacus.ut@protonmail.edu</t>
         </is>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>Puglia</t>
+          <t>Viken</t>
         </is>
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>lacinia orci, consectetuer euismod est arcu ac orci. Ut semper</t>
+          <t>dictum sapien. Aenean massa. Integer vitae nibh. Donec est mauris,</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>Julian Robles</t>
+          <t>Adrienne Santos</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>1-405-666-6441</t>
+          <t>(742) 414-6856</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
         <is>
-          <t>nec.euismod@icloud.edu</t>
+          <t>mauris.non.dui@google.com</t>
         </is>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>Ulster</t>
+          <t>Ulyanovsk Oblast</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>Russian Federation</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>dapibus id, blandit at, nisi. Cum sociis natoque penatibus et</t>
+          <t>sem, vitae aliquam eros turpis non enim. Mauris quis turpis</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>Stephen Ellison</t>
+          <t>Connor Willis</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>(775) 386-9421</t>
+          <t>1-615-901-8387</t>
         </is>
       </c>
       <c r="C19" s="0" t="inlineStr">
         <is>
-          <t>enim@protonmail.org</t>
+          <t>sapien.cras.dolor@protonmail.edu</t>
         </is>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>Alajuela</t>
+          <t>Pembrokeshire</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>posuere cubilia Curae Phasellus ornare. Fusce mollis. Duis sit amet</t>
+          <t>pretium et, rutrum non, hendrerit id, ante. Nunc mauris sapien,</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>Uta Hunt</t>
+          <t>Alisa Oneil</t>
         </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>(162) 888-0133</t>
+          <t>1-362-623-4340</t>
         </is>
       </c>
       <c r="C20" s="0" t="inlineStr">
         <is>
-          <t>at.sem@aol.ca</t>
+          <t>ullamcorper@hotmail.couk</t>
         </is>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>Luik</t>
+          <t>Opolskie</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>dolor. Donec fringilla. Donec feugiat metus sit amet ante. Vivamus</t>
+          <t>amet, consectetuer adipiscing elit. Aliquam auctor, velit eget laoreet posuere,</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>Julie Rodgers</t>
+          <t>Malachi Velez</t>
         </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>(732) 528-0402</t>
+          <t>1-830-746-2193</t>
         </is>
       </c>
       <c r="C21" s="0" t="inlineStr">
         <is>
-          <t>eget.varius@outlook.org</t>
+          <t>lorem.ipsum@aol.net</t>
         </is>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>Carinthia</t>
+          <t>Zeeland</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t>lorem lorem, luctus ut, pellentesque eget, dictum placerat, augue. Sed</t>
+          <t>a nunc. In at pede. Cras vulputate velit eu sem.</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>Callie Russell</t>
+          <t>Ivana Best</t>
         </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>1-281-734-7873</t>
+          <t>1-963-844-3676</t>
         </is>
       </c>
       <c r="C22" s="0" t="inlineStr">
         <is>
-          <t>sapien.cras.dolor@google.net</t>
+          <t>eget@aol.couk</t>
         </is>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>Western Cape</t>
+          <t>Liguria</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t>Etiam bibendum fermentum metus. Aenean sed pede nec ante blandit</t>
+          <t>Vivamus nibh dolor, nonummy ac, feugiat non, lobortis quis, pede.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>Sylvia York</t>
+          <t>Breanna Morrow</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>1-858-428-1126</t>
+          <t>(571) 524-5134</t>
         </is>
       </c>
       <c r="C23" s="0" t="inlineStr">
         <is>
-          <t>phasellus@protonmail.couk</t>
+          <t>natoque@aol.org</t>
         </is>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>łódzkie</t>
+          <t>Tuyên Quang</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>lorem vitae odio sagittis semper. Nam tempor diam dictum sapien.</t>
+          <t>in, cursus et, eros. Proin ultrices. Duis volutpat nunc sit</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>Eve Tate</t>
+          <t>Salvador Whitaker</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>1-107-344-6528</t>
+          <t>1-146-335-5316</t>
         </is>
       </c>
       <c r="C24" s="0" t="inlineStr">
         <is>
-          <t>non.ante@google.org</t>
+          <t>tortor@google.couk</t>
         </is>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>North-East Region</t>
+          <t>Campania</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>vulputate, risus a ultricies adipiscing, enim mi tempor lorem, eget</t>
+          <t>ligula tortor, dictum eu, placerat eget, venenatis a, magna. Lorem</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>Declan Wynn</t>
+          <t>Jared Holcomb</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>1-783-735-7212</t>
+          <t>(799) 207-3672</t>
         </is>
       </c>
       <c r="C25" s="0" t="inlineStr">
         <is>
-          <t>ante@outlook.edu</t>
+          <t>nulla.at@icloud.couk</t>
         </is>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>Xīnán</t>
+          <t>Heredia</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>convallis est, vitae sodales nisi magna sed dui. Fusce aliquam,</t>
+          <t>mollis vitae, posuere at, velit. Cras lorem lorem, luctus ut,</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>Alexandra Ortega</t>
+          <t>Claire Rhodes</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>(304) 640-8041</t>
+          <t>1-865-111-1747</t>
         </is>
       </c>
       <c r="C26" s="0" t="inlineStr">
         <is>
-          <t>non@hotmail.org</t>
+          <t>vel.sapien@aol.couk</t>
         </is>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>Hampshire</t>
+          <t>Schleswig-Holstein</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>mauris elit, dictum eu, eleifend nec, malesuada ut, sem. Nulla</t>
+          <t>consequat enim diam vel arcu. Curabitur ut odio vel est</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>Lillith Blackwell</t>
+          <t>Aspen Robbins</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>(675) 296-0167</t>
+          <t>(112) 964-6836</t>
         </is>
       </c>
       <c r="C27" s="0" t="inlineStr">
         <is>
-          <t>pede.ultrices.a@outlook.couk</t>
+          <t>scelerisque@outlook.edu</t>
         </is>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>Puntarenas</t>
+          <t>Morayshire</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>orci luctus et ultrices posuere cubilia Curae Phasellus ornare. Fusce</t>
+          <t>augue porttitor interdum. Sed auctor odio a purus. Duis elementum,</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>Trevor Lloyd</t>
+          <t>Noel Hopkins</t>
         </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>1-524-415-6377</t>
+          <t>1-357-924-4337</t>
         </is>
       </c>
       <c r="C28" s="0" t="inlineStr">
         <is>
-          <t>turpis@aol.net</t>
+          <t>pede.nec@outlook.net</t>
         </is>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>South Island</t>
+          <t>Waals-Brabant</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
-          <t>nascetur ridiculus mus. Aenean eget magna. Suspendisse tristique neque venenatis</t>
+          <t>Cras dictum ultricies ligula. Nullam enim. Sed nulla ante, iaculis</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>Cassandra Harmon</t>
+          <t>Naomi Berg</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>(383) 821-3552</t>
+          <t>1-877-595-3654</t>
         </is>
       </c>
       <c r="C29" s="0" t="inlineStr">
         <is>
-          <t>sem.ut@aol.com</t>
+          <t>elit@protonmail.edu</t>
         </is>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>Salzburg</t>
+          <t>Murcia</t>
         </is>
       </c>
       <c r="E29" s="0" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t>Nunc sollicitudin commodo ipsum. Suspendisse non leo. Vivamus nibh dolor,</t>
+          <t>Nunc pulvinar arcu et pede. Nunc sed orci lobortis augue</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>Nolan Trujillo</t>
+          <t>Nash Foreman</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>1-526-527-2165</t>
+          <t>1-244-825-5275</t>
         </is>
       </c>
       <c r="C30" s="0" t="inlineStr">
         <is>
-          <t>ac.mattis@aol.couk</t>
+          <t>dolor.dolor.tempus@yahoo.com</t>
         </is>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>Australian Capital Territory</t>
+          <t>Şanlıurfa</t>
         </is>
       </c>
       <c r="E30" s="0" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
-          <t>magnis dis parturient montes, nascetur ridiculus mus. Donec dignissim magna</t>
+          <t>dolor. Fusce feugiat. Lorem ipsum dolor sit amet, consectetuer adipiscing</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>Lawrence Vazquez</t>
+          <t>Avram Avila</t>
         </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>(313) 728-2505</t>
+          <t>1-124-452-1437</t>
         </is>
       </c>
       <c r="C31" s="0" t="inlineStr">
         <is>
-          <t>sociis.natoque@protonmail.edu</t>
+          <t>tincidunt.adipiscing.mauris@hotmail.edu</t>
         </is>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>Rogaland</t>
+          <t>Jammu and Kashmir</t>
         </is>
       </c>
       <c r="E31" s="0" t="inlineStr">
@@ -1069,29 +1069,29 @@
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
-          <t>ultricies ligula. Nullam enim. Sed nulla ante, iaculis nec, eleifend</t>
+          <t>in sodales elit erat vitae risus. Duis a mi fringilla</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>Ashely Strickland</t>
+          <t>Courtney Griffith</t>
         </is>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>1-585-839-2664</t>
+          <t>1-964-494-1347</t>
         </is>
       </c>
       <c r="C32" s="0" t="inlineStr">
         <is>
-          <t>nisi.aenean@icloud.org</t>
+          <t>duis.gravida@yahoo.ca</t>
         </is>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>Vestland</t>
+          <t>Maranhão</t>
         </is>
       </c>
       <c r="E32" s="0" t="inlineStr">
@@ -1101,669 +1101,669 @@
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
-          <t>mauris, aliquam eu, accumsan sed, facilisis vitae, orci. Phasellus dapibus</t>
+          <t>tellus non magna. Nam ligula elit, pretium et, rutrum non,</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>Lucy Macdonald</t>
+          <t>Tashya Alston</t>
         </is>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>(828) 615-5335</t>
+          <t>1-318-313-8211</t>
         </is>
       </c>
       <c r="C33" s="0" t="inlineStr">
         <is>
-          <t>phasellus@icloud.org</t>
+          <t>varius.orci@google.org</t>
         </is>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>Namen</t>
+          <t>Khyber Pakhtoonkhwa</t>
         </is>
       </c>
       <c r="E33" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
-          <t>id, mollis nec, cursus a, enim. Suspendisse aliquet, sem ut</t>
+          <t>vulputate dui, nec tempus mauris erat eget ipsum. Suspendisse sagittis.</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>Duncan Fletcher</t>
+          <t>Nigel Hodges</t>
         </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>1-986-936-5647</t>
+          <t>1-641-242-6044</t>
         </is>
       </c>
       <c r="C34" s="0" t="inlineStr">
         <is>
-          <t>maecenas@outlook.org</t>
+          <t>at.risus@protonmail.com</t>
         </is>
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t>Junín</t>
+          <t>Flevoland</t>
         </is>
       </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
-          <t>vehicula risus. Nulla eget metus eu erat semper rutrum. Fusce</t>
+          <t>sed pede nec ante blandit viverra. Donec tempus, lorem fringilla</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>Ciaran Webster</t>
+          <t>Echo Watkins</t>
         </is>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>1-422-476-2256</t>
+          <t>(433) 217-2128</t>
         </is>
       </c>
       <c r="C35" s="0" t="inlineStr">
         <is>
-          <t>ac.tellus@google.org</t>
+          <t>eu.nibh@hotmail.ca</t>
         </is>
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
-          <t>Bali</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E35" s="0" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
-          <t>primis in faucibus orci luctus et ultrices posuere cubilia Curae</t>
+          <t>Etiam bibendum fermentum metus. Aenean sed pede nec ante blandit</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>Chester Stark</t>
+          <t>Jana Woods</t>
         </is>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>1-752-658-4901</t>
+          <t>1-323-483-7567</t>
         </is>
       </c>
       <c r="C36" s="0" t="inlineStr">
         <is>
-          <t>at@protonmail.com</t>
+          <t>dapibus@icloud.couk</t>
         </is>
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
-          <t>North Island</t>
+          <t>Huádōng</t>
         </is>
       </c>
       <c r="E36" s="0" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F36" s="0" t="inlineStr">
         <is>
-          <t>et, rutrum non, hendrerit id, ante. Nunc mauris sapien, cursus</t>
+          <t>natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus.</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>Maxwell Head</t>
+          <t>Hop Frye</t>
         </is>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>(932) 572-5281</t>
+          <t>1-953-464-7173</t>
         </is>
       </c>
       <c r="C37" s="0" t="inlineStr">
         <is>
-          <t>aliquam.erat@yahoo.ca</t>
+          <t>gravida.mauris@hotmail.com</t>
         </is>
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
-          <t>Stirlingshire</t>
+          <t>Viken</t>
         </is>
       </c>
       <c r="E37" s="0" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
-          <t>vel pede blandit congue. In scelerisque scelerisque dui. Suspendisse ac</t>
+          <t>Nunc ullamcorper, velit in aliquet lobortis, nisi nibh lacinia orci,</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>Velma Zimmerman</t>
+          <t>Carissa Slater</t>
         </is>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>(672) 617-4786</t>
+          <t>1-782-360-2678</t>
         </is>
       </c>
       <c r="C38" s="0" t="inlineStr">
         <is>
-          <t>convallis.erat.eget@aol.edu</t>
+          <t>nulla.integer.urna@yahoo.net</t>
         </is>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
-          <t>Leinster</t>
+          <t>Upper Austria</t>
         </is>
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
         <is>
-          <t>nibh. Aliquam ornare, libero at auctor ullamcorper, nisl arcu iaculis</t>
+          <t>tellus eu augue porttitor interdum. Sed auctor odio a purus.</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>Ciaran George</t>
+          <t>Rachel Meyers</t>
         </is>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>1-386-241-8819</t>
+          <t>(764) 535-8528</t>
         </is>
       </c>
       <c r="C39" s="0" t="inlineStr">
         <is>
-          <t>elit.elit@google.com</t>
+          <t>eleifend@yahoo.org</t>
         </is>
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
-          <t>Auvergne</t>
+          <t>Sinaloa</t>
         </is>
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F39" s="0" t="inlineStr">
         <is>
-          <t>Nulla semper tellus id nunc interdum feugiat. Sed nec metus</t>
+          <t>tellus sem mollis dui, in sodales elit erat vitae risus.</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>Hedley Goodman</t>
+          <t>Audrey Page</t>
         </is>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>(963) 725-3135</t>
+          <t>(699) 822-8596</t>
         </is>
       </c>
       <c r="C40" s="0" t="inlineStr">
         <is>
-          <t>tincidunt.nibh@outlook.couk</t>
+          <t>nec.ligula@protonmail.net</t>
         </is>
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
-          <t>South Jeolla</t>
+          <t>Tamil Nadu</t>
         </is>
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="F40" s="0" t="inlineStr">
         <is>
-          <t>dui nec urna suscipit nonummy. Fusce fermentum fermentum arcu. Vestibulum</t>
+          <t>hendrerit. Donec porttitor tellus non magna. Nam ligula elit, pretium</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>Malachi Vasquez</t>
+          <t>Carlos Knight</t>
         </is>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>1-508-719-7557</t>
+          <t>1-549-374-4834</t>
         </is>
       </c>
       <c r="C41" s="0" t="inlineStr">
         <is>
-          <t>cras.pellentesque@aol.org</t>
+          <t>duis@yahoo.org</t>
         </is>
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>Styria</t>
         </is>
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
         <is>
-          <t>Curae Phasellus ornare. Fusce mollis. Duis sit amet diam eu</t>
+          <t>lorem, eget mollis lectus pede et risus. Quisque libero lacus,</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>Leilani Contreras</t>
+          <t>Aurelia Hull</t>
         </is>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>1-535-773-6758</t>
+          <t>1-460-798-7577</t>
         </is>
       </c>
       <c r="C42" s="0" t="inlineStr">
         <is>
-          <t>a.arcu@protonmail.org</t>
+          <t>etiam.gravida@yahoo.com</t>
         </is>
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
-          <t>Gauteng</t>
+          <t>Friuli-Venezia Giulia</t>
         </is>
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="F42" s="0" t="inlineStr">
         <is>
-          <t>augue, eu tempor erat neque non quam. Pellentesque habitant morbi</t>
+          <t>lectus, a sollicitudin orci sem eget massa. Suspendisse eleifend. Cras</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>Seth Vasquez</t>
+          <t>Eugenia Fitzgerald</t>
         </is>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>(288) 846-2250</t>
+          <t>1-662-608-7648</t>
         </is>
       </c>
       <c r="C43" s="0" t="inlineStr">
         <is>
-          <t>et@aol.net</t>
+          <t>ullamcorper@outlook.ca</t>
         </is>
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
-          <t>Podkarpackie</t>
+          <t>Lima</t>
         </is>
       </c>
       <c r="E43" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
-          <t>libero. Donec consectetuer mauris id sapien. Cras dolor dolor, tempus</t>
+          <t>mi lorem, vehicula et, rutrum eu, ultrices sit amet, risus.</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>Octavia Short</t>
+          <t>Geoffrey Sherman</t>
         </is>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>(352) 526-3226</t>
+          <t>1-281-263-9907</t>
         </is>
       </c>
       <c r="C44" s="0" t="inlineStr">
         <is>
-          <t>a.sollicitudin@icloud.ca</t>
+          <t>nonummy.ipsum@yahoo.ca</t>
         </is>
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
-          <t>Cordillera Administrative Region</t>
+          <t>Antofagasta</t>
         </is>
       </c>
       <c r="E44" s="0" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
-          <t>ornare. Fusce mollis. Duis sit amet diam eu dolor egestas</t>
+          <t>risus. Nunc ac sem ut dolor dapibus gravida. Aliquam tincidunt,</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>Stephen Becker</t>
+          <t>Tanner Barber</t>
         </is>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>(486) 655-8851</t>
+          <t>1-706-323-3846</t>
         </is>
       </c>
       <c r="C45" s="0" t="inlineStr">
         <is>
-          <t>vel.arcu@outlook.com</t>
+          <t>risus.quis@outlook.net</t>
         </is>
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
-          <t>Munster</t>
+          <t>Namen</t>
         </is>
       </c>
       <c r="E45" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F45" s="0" t="inlineStr">
         <is>
-          <t>nec quam. Curabitur vel lectus. Cum sociis natoque penatibus et</t>
+          <t>Integer sem elit, pharetra ut, pharetra sed, hendrerit a, arcu.</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>Deacon Hines</t>
+          <t>Rahim Huber</t>
         </is>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>1-633-878-3252</t>
+          <t>1-841-641-1266</t>
         </is>
       </c>
       <c r="C46" s="0" t="inlineStr">
         <is>
-          <t>urna.justo.faucibus@icloud.ca</t>
+          <t>gravida.praesent.eu@protonmail.com</t>
         </is>
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
-          <t>Pondicherry</t>
+          <t>Zuid Holland</t>
         </is>
       </c>
       <c r="E46" s="0" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F46" s="0" t="inlineStr">
         <is>
-          <t>Mauris nulla. Integer urna. Vivamus molestie dapibus ligula. Aliquam erat</t>
+          <t>egestas. Aliquam fringilla cursus purus. Nullam scelerisque neque sed sem</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>Teagan Vaughn</t>
+          <t>Rina Massey</t>
         </is>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>1-395-234-0922</t>
+          <t>1-578-315-5891</t>
         </is>
       </c>
       <c r="C47" s="0" t="inlineStr">
         <is>
-          <t>neque.non@google.net</t>
+          <t>iaculis.aliquet.diam@google.com</t>
         </is>
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
-          <t>Murcia</t>
+          <t>Małopolskie</t>
         </is>
       </c>
       <c r="E47" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>purus sapien, gravida non, sollicitudin a, malesuada id, erat. Etiam</t>
+          <t>vel, convallis in, cursus et, eros. Proin ultrices. Duis volutpat</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>Savannah Reed</t>
+          <t>Branden Hanson</t>
         </is>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>1-386-232-5643</t>
+          <t>1-435-872-0877</t>
         </is>
       </c>
       <c r="C48" s="0" t="inlineStr">
         <is>
-          <t>ornare.tortor.at@hotmail.ca</t>
+          <t>ridiculus@yahoo.ca</t>
         </is>
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
-          <t>Oost-Vlaanderen</t>
+          <t>São Paulo</t>
         </is>
       </c>
       <c r="E48" s="0" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t>euismod et, commodo at, libero. Morbi accumsan laoreet ipsum. Curabitur</t>
+          <t>augue. Sed molestie. Sed id risus quis diam luctus lobortis.</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>Zachery Martinez</t>
+          <t>Chava Jennings</t>
         </is>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>(898) 264-0274</t>
+          <t>1-892-754-0688</t>
         </is>
       </c>
       <c r="C49" s="0" t="inlineStr">
         <is>
-          <t>nec.euismod.in@icloud.edu</t>
+          <t>consequat.nec@aol.edu</t>
         </is>
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
-          <t>Sachsen</t>
+          <t>Jigawa</t>
         </is>
       </c>
       <c r="E49" s="0" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F49" s="0" t="inlineStr">
         <is>
-          <t>lectus convallis est, vitae sodales nisi magna sed dui. Fusce</t>
+          <t>malesuada malesuada. Integer id magna et ipsum cursus vestibulum. Mauris</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>Alea Morton</t>
+          <t>Carissa Stewart</t>
         </is>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>1-814-533-6328</t>
+          <t>(313) 134-2198</t>
         </is>
       </c>
       <c r="C50" s="0" t="inlineStr">
         <is>
-          <t>mauris.blandit.enim@protonmail.couk</t>
+          <t>at.arcu@google.org</t>
         </is>
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
-          <t>Extremadura</t>
+          <t>Vorarlberg</t>
         </is>
       </c>
       <c r="E50" s="0" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F50" s="0" t="inlineStr">
         <is>
-          <t>arcu iaculis enim, sit amet ornare lectus justo eu arcu.</t>
+          <t>libero. Proin sed turpis nec mauris blandit mattis. Cras eget</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>Briar Guerrero</t>
+          <t>Dexter Suarez</t>
         </is>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>1-673-372-5823</t>
+          <t>1-446-863-4381</t>
         </is>
       </c>
       <c r="C51" s="0" t="inlineStr">
         <is>
-          <t>pellentesque.sed.dictum@google.edu</t>
+          <t>nibh.aliquam.ornare@aol.couk</t>
         </is>
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
-          <t>Belgorod Oblast</t>
+          <t>Provence-Alpes-Côte d'Azur</t>
         </is>
       </c>
       <c r="E51" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>amet nulla. Donec non justo. Proin non massa non ante</t>
+          <t>Cras dolor dolor, tempus non, lacinia at, iaculis quis, pede.</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>Moses Rhodes</t>
+          <t>Marshall Carrillo</t>
         </is>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>(551) 234-8225</t>
+          <t>1-445-476-9220</t>
         </is>
       </c>
       <c r="C52" s="0" t="inlineStr">
         <is>
-          <t>pharetra.nibh.aliquam@protonmail.ca</t>
+          <t>lacinia@protonmail.com</t>
         </is>
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
-          <t>Trøndelag</t>
+          <t>Mexico City</t>
         </is>
       </c>
       <c r="E52" s="0" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="F52" s="0" t="inlineStr">
         <is>
-          <t>dignissim magna a tortor. Nunc commodo auctor velit. Aliquam nisl.</t>
+          <t>velit justo nec ante. Maecenas mi felis, adipiscing fringilla, porttitor</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>Brooke Boone</t>
+          <t>Jameson Glass</t>
         </is>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
-          <t>(727) 463-7378</t>
+          <t>1-721-569-5615</t>
         </is>
       </c>
       <c r="C53" s="0" t="inlineStr">
         <is>
-          <t>dui@google.com</t>
+          <t>commodo.hendrerit@aol.net</t>
         </is>
       </c>
       <c r="D53" s="0" t="inlineStr">
         <is>
-          <t>Andalucía</t>
+          <t>Tyrol</t>
         </is>
       </c>
       <c r="E53" s="0" t="inlineStr">
@@ -1773,1543 +1773,1543 @@
       </c>
       <c r="F53" s="0" t="inlineStr">
         <is>
-          <t>dolor dapibus gravida. Aliquam tincidunt, nunc ac mattis ornare, lectus</t>
+          <t>eget magna. Suspendisse tristique neque venenatis lacus. Etiam bibendum fermentum</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>Charity Goodwin</t>
+          <t>Yuli Jennings</t>
         </is>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>(721) 208-1815</t>
+          <t>1-476-418-7568</t>
         </is>
       </c>
       <c r="C54" s="0" t="inlineStr">
         <is>
-          <t>aliquam.arcu@google.org</t>
+          <t>molestie.arcu.sed@aol.com</t>
         </is>
       </c>
       <c r="D54" s="0" t="inlineStr">
         <is>
-          <t>Norfolk</t>
+          <t>Limburg</t>
         </is>
       </c>
       <c r="E54" s="0" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t>venenatis lacus. Etiam bibendum fermentum metus. Aenean sed pede nec</t>
+          <t>augue ac ipsum. Phasellus vitae mauris sit amet lorem semper</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>Erin Ellison</t>
+          <t>Heidi Good</t>
         </is>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>(871) 665-8596</t>
+          <t>1-335-430-5385</t>
         </is>
       </c>
       <c r="C55" s="0" t="inlineStr">
         <is>
-          <t>ac@icloud.edu</t>
+          <t>nulla.eget@icloud.net</t>
         </is>
       </c>
       <c r="D55" s="0" t="inlineStr">
         <is>
-          <t>Møre og Romsdal</t>
+          <t>Western Australia</t>
         </is>
       </c>
       <c r="E55" s="0" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
-          <t>elit. Etiam laoreet, libero et tristique pellentesque, tellus sem mollis</t>
+          <t>magna nec quam. Curabitur vel lectus. Cum sociis natoque penatibus</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>Candace Watson</t>
+          <t>Jackson Walsh</t>
         </is>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
-          <t>(486) 452-3774</t>
+          <t>(643) 861-8241</t>
         </is>
       </c>
       <c r="C56" s="0" t="inlineStr">
         <is>
-          <t>mauris.integer@yahoo.ca</t>
+          <t>pharetra@hotmail.couk</t>
         </is>
       </c>
       <c r="D56" s="0" t="inlineStr">
         <is>
-          <t>Tamaulipas</t>
+          <t>Xīnán</t>
         </is>
       </c>
       <c r="E56" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
-          <t>nisi a odio semper cursus. Integer mollis. Integer tincidunt aliquam</t>
+          <t>Duis dignissim tempor arcu. Vestibulum ut eros non enim commodo</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>Dalton Whitfield</t>
+          <t>Rhea Bryan</t>
         </is>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
-          <t>(316) 161-3838</t>
+          <t>1-106-445-4638</t>
         </is>
       </c>
       <c r="C57" s="0" t="inlineStr">
         <is>
-          <t>fusce.aliquam.enim@hotmail.com</t>
+          <t>amet.faucibus.ut@hotmail.net</t>
         </is>
       </c>
       <c r="D57" s="0" t="inlineStr">
         <is>
-          <t>Ulyanovsk Oblast</t>
+          <t>Kogi</t>
         </is>
       </c>
       <c r="E57" s="0" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="F57" s="0" t="inlineStr">
         <is>
-          <t>purus. Nullam scelerisque neque sed sem egestas blandit. Nam nulla</t>
+          <t>diam nunc, ullamcorper eu, euismod ac, fermentum vel, mauris. Integer</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>Skyler Gordon</t>
+          <t>Sarah Garcia</t>
         </is>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
-          <t>(770) 644-1680</t>
+          <t>1-412-471-4014</t>
         </is>
       </c>
       <c r="C58" s="0" t="inlineStr">
         <is>
-          <t>risus.quis.diam@outlook.couk</t>
+          <t>curabitur@hotmail.org</t>
         </is>
       </c>
       <c r="D58" s="0" t="inlineStr">
         <is>
-          <t>Rogaland</t>
+          <t>Mecklenburg-Vorpommern</t>
         </is>
       </c>
       <c r="E58" s="0" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F58" s="0" t="inlineStr">
         <is>
-          <t>risus odio, auctor vitae, aliquet nec, imperdiet nec, leo. Morbi</t>
+          <t>lacinia at, iaculis quis, pede. Praesent eu dui. Cum sociis</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>Allegra Franks</t>
+          <t>Mallory Hunter</t>
         </is>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
-          <t>(557) 921-9325</t>
+          <t>1-652-411-5782</t>
         </is>
       </c>
       <c r="C59" s="0" t="inlineStr">
         <is>
-          <t>eget.tincidunt@aol.couk</t>
+          <t>litora.torquent@outlook.edu</t>
         </is>
       </c>
       <c r="D59" s="0" t="inlineStr">
         <is>
-          <t>South Island</t>
+          <t>Rivne oblast</t>
         </is>
       </c>
       <c r="E59" s="0" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F59" s="0" t="inlineStr">
         <is>
-          <t>dolor. Nulla semper tellus id nunc interdum feugiat. Sed nec</t>
+          <t>ac turpis egestas. Fusce aliquet magna a neque. Nullam ut</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>Blaze Lucas</t>
+          <t>Xyla Walton</t>
         </is>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
-          <t>1-565-625-8336</t>
+          <t>1-854-229-1260</t>
         </is>
       </c>
       <c r="C60" s="0" t="inlineStr">
         <is>
-          <t>nam.tempor@hotmail.edu</t>
+          <t>aliquam.eu@protonmail.edu</t>
         </is>
       </c>
       <c r="D60" s="0" t="inlineStr">
         <is>
-          <t>Hòa Bình</t>
+          <t>British Columbia</t>
         </is>
       </c>
       <c r="E60" s="0" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F60" s="0" t="inlineStr">
         <is>
-          <t>non enim commodo hendrerit. Donec porttitor tellus non magna. Nam</t>
+          <t>nisi magna sed dui. Fusce aliquam, enim nec tempus scelerisque,</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>Ferris Morales</t>
+          <t>Cleo Chen</t>
         </is>
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
-          <t>1-775-257-3823</t>
+          <t>(753) 487-4184</t>
         </is>
       </c>
       <c r="C61" s="0" t="inlineStr">
         <is>
-          <t>nisl@icloud.net</t>
+          <t>libero.et@yahoo.ca</t>
         </is>
       </c>
       <c r="D61" s="0" t="inlineStr">
         <is>
-          <t>Alajuela</t>
+          <t>Västra Götalands län</t>
         </is>
       </c>
       <c r="E61" s="0" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F61" s="0" t="inlineStr">
         <is>
-          <t>eu turpis. Nulla aliquet. Proin velit. Sed malesuada augue ut</t>
+          <t>ac mattis ornare, lectus ante dictum mi, ac mattis velit</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>Ferris Patterson</t>
+          <t>Ulric Davidson</t>
         </is>
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
-          <t>1-472-281-8530</t>
+          <t>(669) 771-3826</t>
         </is>
       </c>
       <c r="C62" s="0" t="inlineStr">
         <is>
-          <t>nonummy.fusce@protonmail.ca</t>
+          <t>donec.nibh@hotmail.couk</t>
         </is>
       </c>
       <c r="D62" s="0" t="inlineStr">
         <is>
-          <t>Western Visayas</t>
+          <t>Tabasco</t>
         </is>
       </c>
       <c r="E62" s="0" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="F62" s="0" t="inlineStr">
         <is>
-          <t>nisi a odio semper cursus. Integer mollis. Integer tincidunt aliquam</t>
+          <t>dictum sapien. Aenean massa. Integer vitae nibh. Donec est mauris,</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>Galvin Mayer</t>
+          <t>Hayes Evans</t>
         </is>
       </c>
       <c r="B63" s="0" t="inlineStr">
         <is>
-          <t>(247) 705-1977</t>
+          <t>1-807-694-2452</t>
         </is>
       </c>
       <c r="C63" s="0" t="inlineStr">
         <is>
-          <t>dui.in@google.com</t>
+          <t>cursus.integer@google.couk</t>
         </is>
       </c>
       <c r="D63" s="0" t="inlineStr">
         <is>
-          <t>Queensland</t>
+          <t>Schleswig-Holstein</t>
         </is>
       </c>
       <c r="E63" s="0" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F63" s="0" t="inlineStr">
         <is>
-          <t>lorem, eget mollis lectus pede et risus. Quisque libero lacus,</t>
+          <t>elit. Nulla facilisi. Sed neque. Sed eget lacus. Mauris non</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>Abel Bruce</t>
+          <t>Ariel Hendricks</t>
         </is>
       </c>
       <c r="B64" s="0" t="inlineStr">
         <is>
-          <t>1-831-875-8151</t>
+          <t>(988) 771-4697</t>
         </is>
       </c>
       <c r="C64" s="0" t="inlineStr">
         <is>
-          <t>egestas.duis.ac@icloud.net</t>
+          <t>tristique.senectus@yahoo.org</t>
         </is>
       </c>
       <c r="D64" s="0" t="inlineStr">
         <is>
-          <t>Bengkulu</t>
+          <t>Northern Cape</t>
         </is>
       </c>
       <c r="E64" s="0" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F64" s="0" t="inlineStr">
         <is>
-          <t>sem, vitae aliquam eros turpis non enim. Mauris quis turpis</t>
+          <t>penatibus et magnis dis parturient montes, nascetur ridiculus mus. Proin</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>Myles Graves</t>
+          <t>Irma Becker</t>
         </is>
       </c>
       <c r="B65" s="0" t="inlineStr">
         <is>
-          <t>(258) 664-9626</t>
+          <t>1-377-149-1673</t>
         </is>
       </c>
       <c r="C65" s="0" t="inlineStr">
         <is>
-          <t>libero.lacus@protonmail.couk</t>
+          <t>tempus.eu.ligula@google.edu</t>
         </is>
       </c>
       <c r="D65" s="0" t="inlineStr">
         <is>
-          <t>Coquimbo</t>
+          <t>Chocó</t>
         </is>
       </c>
       <c r="E65" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F65" s="0" t="inlineStr">
         <is>
-          <t>lorem fringilla ornare placerat, orci lacus vestibulum lorem, sit amet</t>
+          <t>Cras eget nisi dictum augue malesuada malesuada. Integer id magna</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>Olivia Shaffer</t>
+          <t>Lara Cross</t>
         </is>
       </c>
       <c r="B66" s="0" t="inlineStr">
         <is>
-          <t>1-473-567-5314</t>
+          <t>1-572-726-2481</t>
         </is>
       </c>
       <c r="C66" s="0" t="inlineStr">
         <is>
-          <t>phasellus.dolor@google.org</t>
+          <t>scelerisque.mollis@yahoo.org</t>
         </is>
       </c>
       <c r="D66" s="0" t="inlineStr">
         <is>
-          <t>Ulster</t>
+          <t>Tula Oblast</t>
         </is>
       </c>
       <c r="E66" s="0" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F66" s="0" t="inlineStr">
         <is>
-          <t>eu, accumsan sed, facilisis vitae, orci. Phasellus dapibus quam quis</t>
+          <t>magna et ipsum cursus vestibulum. Mauris magna. Duis dignissim tempor</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>Paula Morton</t>
+          <t>Mufutau Greer</t>
         </is>
       </c>
       <c r="B67" s="0" t="inlineStr">
         <is>
-          <t>1-262-816-5090</t>
+          <t>1-588-748-5168</t>
         </is>
       </c>
       <c r="C67" s="0" t="inlineStr">
         <is>
-          <t>venenatis.a.magna@yahoo.org</t>
+          <t>fringilla.est@yahoo.org</t>
         </is>
       </c>
       <c r="D67" s="0" t="inlineStr">
         <is>
-          <t>Zeeland</t>
+          <t>North Sumatra</t>
         </is>
       </c>
       <c r="E67" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F67" s="0" t="inlineStr">
         <is>
-          <t>aliquet libero. Integer in magna. Phasellus dolor elit, pellentesque a,</t>
+          <t>adipiscing. Mauris molestie pharetra nibh. Aliquam ornare, libero at auctor</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>Barbara Ball</t>
+          <t>Kameko Foster</t>
         </is>
       </c>
       <c r="B68" s="0" t="inlineStr">
         <is>
-          <t>1-107-557-0096</t>
+          <t>1-672-844-0763</t>
         </is>
       </c>
       <c r="C68" s="0" t="inlineStr">
         <is>
-          <t>mattis.velit.justo@protonmail.net</t>
+          <t>duis.risus@outlook.ca</t>
         </is>
       </c>
       <c r="D68" s="0" t="inlineStr">
         <is>
-          <t>North Island</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="E68" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F68" s="0" t="inlineStr">
         <is>
-          <t>neque sed dictum eleifend, nunc risus varius orci, in consequat</t>
+          <t>id nunc interdum feugiat. Sed nec metus facilisis lorem tristique</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>Tatiana Ball</t>
+          <t>Jana Lamb</t>
         </is>
       </c>
       <c r="B69" s="0" t="inlineStr">
         <is>
-          <t>(339) 587-6448</t>
+          <t>1-627-658-2668</t>
         </is>
       </c>
       <c r="C69" s="0" t="inlineStr">
         <is>
-          <t>vel.venenatis@protonmail.net</t>
+          <t>non.bibendum.sed@yahoo.com</t>
         </is>
       </c>
       <c r="D69" s="0" t="inlineStr">
         <is>
-          <t>West Region</t>
+          <t>Bình Định</t>
         </is>
       </c>
       <c r="E69" s="0" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F69" s="0" t="inlineStr">
         <is>
-          <t>aliquet vel, vulputate eu, odio. Phasellus at augue id ante</t>
+          <t>tristique senectus et netus et malesuada fames ac turpis egestas.</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>Martena Poole</t>
+          <t>David Watts</t>
         </is>
       </c>
       <c r="B70" s="0" t="inlineStr">
         <is>
-          <t>(711) 238-5361</t>
+          <t>1-551-263-8428</t>
         </is>
       </c>
       <c r="C70" s="0" t="inlineStr">
         <is>
-          <t>libero.lacus@icloud.com</t>
+          <t>quis.turpis@icloud.ca</t>
         </is>
       </c>
       <c r="D70" s="0" t="inlineStr">
         <is>
-          <t>Paraná</t>
+          <t>Magadan Oblast</t>
         </is>
       </c>
       <c r="E70" s="0" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F70" s="0" t="inlineStr">
         <is>
-          <t>elementum sem, vitae aliquam eros turpis non enim. Mauris quis</t>
+          <t>egestas hendrerit neque. In ornare sagittis felis. Donec tempor, est</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>Cruz Battle</t>
+          <t>Whitney Forbes</t>
         </is>
       </c>
       <c r="B71" s="0" t="inlineStr">
         <is>
-          <t>(112) 945-7156</t>
+          <t>1-807-564-5527</t>
         </is>
       </c>
       <c r="C71" s="0" t="inlineStr">
         <is>
-          <t>mollis.non.cursus@protonmail.com</t>
+          <t>maecenas.mi@google.couk</t>
         </is>
       </c>
       <c r="D71" s="0" t="inlineStr">
         <is>
-          <t>Navarra</t>
+          <t>FATA</t>
         </is>
       </c>
       <c r="E71" s="0" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F71" s="0" t="inlineStr">
         <is>
-          <t>cursus in, hendrerit consectetuer, cursus et, magna. Praesent interdum ligula</t>
+          <t>eget metus eu erat semper rutrum. Fusce dolor quam, elementum</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>Nyssa Mullins</t>
+          <t>Lysandra Salas</t>
         </is>
       </c>
       <c r="B72" s="0" t="inlineStr">
         <is>
-          <t>(728) 229-1820</t>
+          <t>1-554-384-3169</t>
         </is>
       </c>
       <c r="C72" s="0" t="inlineStr">
         <is>
-          <t>erat.etiam.vestibulum@protonmail.couk</t>
+          <t>nec.ante@yahoo.org</t>
         </is>
       </c>
       <c r="D72" s="0" t="inlineStr">
         <is>
-          <t>Östergötlands län</t>
+          <t>Illes Balears</t>
         </is>
       </c>
       <c r="E72" s="0" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F72" s="0" t="inlineStr">
         <is>
-          <t>penatibus et magnis dis parturient montes, nascetur ridiculus mus. Proin</t>
+          <t>ullamcorper. Duis cursus, diam at pretium aliquet, metus urna convallis</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>Wendy Foley</t>
+          <t>Jin White</t>
         </is>
       </c>
       <c r="B73" s="0" t="inlineStr">
         <is>
-          <t>1-424-287-9732</t>
+          <t>1-354-281-1488</t>
         </is>
       </c>
       <c r="C73" s="0" t="inlineStr">
         <is>
-          <t>sit.amet@yahoo.couk</t>
+          <t>et.magnis.dis@aol.org</t>
         </is>
       </c>
       <c r="D73" s="0" t="inlineStr">
         <is>
-          <t>Thừa Thiên–Huế</t>
+          <t>Queensland</t>
         </is>
       </c>
       <c r="E73" s="0" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F73" s="0" t="inlineStr">
         <is>
-          <t>sollicitudin commodo ipsum. Suspendisse non leo. Vivamus nibh dolor, nonummy</t>
+          <t>euismod et, commodo at, libero. Morbi accumsan laoreet ipsum. Curabitur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>Medge Glass</t>
+          <t>Quynn Blevins</t>
         </is>
       </c>
       <c r="B74" s="0" t="inlineStr">
         <is>
-          <t>(476) 682-2111</t>
+          <t>1-897-374-7724</t>
         </is>
       </c>
       <c r="C74" s="0" t="inlineStr">
         <is>
-          <t>duis.gravida@icloud.ca</t>
+          <t>donec.egestas@hotmail.couk</t>
         </is>
       </c>
       <c r="D74" s="0" t="inlineStr">
         <is>
-          <t>Caraga</t>
+          <t>Provence-Alpes-Côte d'Azur</t>
         </is>
       </c>
       <c r="E74" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="F74" s="0" t="inlineStr">
         <is>
-          <t>euismod ac, fermentum vel, mauris. Integer sem elit, pharetra ut,</t>
+          <t>Nulla aliquet. Proin velit. Sed malesuada augue ut lacus. Nulla</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>Hop Nelson</t>
+          <t>Violet Boone</t>
         </is>
       </c>
       <c r="B75" s="0" t="inlineStr">
         <is>
-          <t>(144) 794-4929</t>
+          <t>(317) 282-1687</t>
         </is>
       </c>
       <c r="C75" s="0" t="inlineStr">
         <is>
-          <t>lectus.rutrum@aol.ca</t>
+          <t>nunc.id@google.couk</t>
         </is>
       </c>
       <c r="D75" s="0" t="inlineStr">
         <is>
-          <t>Bali</t>
+          <t>South Chungcheong</t>
         </is>
       </c>
       <c r="E75" s="0" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F75" s="0" t="inlineStr">
         <is>
-          <t>in, hendrerit consectetuer, cursus et, magna. Praesent interdum ligula eu</t>
+          <t>arcu. Aliquam ultrices iaculis odio. Nam interdum enim non nisi.</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>Ray Leon</t>
+          <t>Carissa Chen</t>
         </is>
       </c>
       <c r="B76" s="0" t="inlineStr">
         <is>
-          <t>(437) 346-8214</t>
+          <t>1-153-774-0622</t>
         </is>
       </c>
       <c r="C76" s="0" t="inlineStr">
         <is>
-          <t>risus.at@aol.couk</t>
+          <t>integer.vitae.nibh@google.couk</t>
         </is>
       </c>
       <c r="D76" s="0" t="inlineStr">
         <is>
-          <t>Minas Gerais</t>
+          <t>Western Australia</t>
         </is>
       </c>
       <c r="E76" s="0" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F76" s="0" t="inlineStr">
         <is>
-          <t>tellus, imperdiet non, vestibulum nec, euismod in, dolor. Fusce feugiat.</t>
+          <t>ante bibendum ullamcorper. Duis cursus, diam at pretium aliquet, metus</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>Eagan Carr</t>
+          <t>Samuel Mcmillan</t>
         </is>
       </c>
       <c r="B77" s="0" t="inlineStr">
         <is>
-          <t>1-103-977-0302</t>
+          <t>(752) 666-5470</t>
         </is>
       </c>
       <c r="C77" s="0" t="inlineStr">
         <is>
-          <t>odio.auctor.vitae@outlook.couk</t>
+          <t>mi.enim@aol.net</t>
         </is>
       </c>
       <c r="D77" s="0" t="inlineStr">
         <is>
-          <t>Ternopil oblast</t>
+          <t>Rheinland-Pfalz</t>
         </is>
       </c>
       <c r="E77" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F77" s="0" t="inlineStr">
         <is>
-          <t>Etiam vestibulum massa rutrum magna. Cras convallis convallis dolor. Quisque</t>
+          <t>fermentum convallis ligula. Donec luctus aliquet odio. Etiam ligula tortor,</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>Lacy Parks</t>
+          <t>Hu Massey</t>
         </is>
       </c>
       <c r="B78" s="0" t="inlineStr">
         <is>
-          <t>1-776-418-6787</t>
+          <t>(412) 623-6779</t>
         </is>
       </c>
       <c r="C78" s="0" t="inlineStr">
         <is>
-          <t>ornare.elit@aol.net</t>
+          <t>metus.vitae@outlook.couk</t>
         </is>
       </c>
       <c r="D78" s="0" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Munster</t>
         </is>
       </c>
       <c r="E78" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="F78" s="0" t="inlineStr">
         <is>
-          <t>Maecenas mi felis, adipiscing fringilla, porttitor vulputate, posuere vulputate, lacus.</t>
+          <t>penatibus et magnis dis parturient montes, nascetur ridiculus mus. Proin</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>Molly Crosby</t>
+          <t>Declan Maxwell</t>
         </is>
       </c>
       <c r="B79" s="0" t="inlineStr">
         <is>
-          <t>1-627-130-0127</t>
+          <t>1-384-897-3631</t>
         </is>
       </c>
       <c r="C79" s="0" t="inlineStr">
         <is>
-          <t>vel@aol.ca</t>
+          <t>consectetuer@aol.com</t>
         </is>
       </c>
       <c r="D79" s="0" t="inlineStr">
         <is>
-          <t>Liguria</t>
+          <t>Limpopo</t>
         </is>
       </c>
       <c r="E79" s="0" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F79" s="0" t="inlineStr">
         <is>
-          <t>magna a neque. Nullam ut nisi a odio semper cursus.</t>
+          <t>pellentesque eget, dictum placerat, augue. Sed molestie. Sed id risus</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>Jada Santana</t>
+          <t>Ryder Ware</t>
         </is>
       </c>
       <c r="B80" s="0" t="inlineStr">
         <is>
-          <t>1-881-767-0155</t>
+          <t>1-412-364-7808</t>
         </is>
       </c>
       <c r="C80" s="0" t="inlineStr">
         <is>
-          <t>consectetuer@google.com</t>
+          <t>vestibulum.accumsan.neque@google.edu</t>
         </is>
       </c>
       <c r="D80" s="0" t="inlineStr">
         <is>
-          <t>South Australia</t>
+          <t>Ulster</t>
         </is>
       </c>
       <c r="E80" s="0" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F80" s="0" t="inlineStr">
         <is>
-          <t>Aenean gravida nunc sed pede. Cum sociis natoque penatibus et</t>
+          <t>vulputate ullamcorper magna. Sed eu eros. Nam consequat dolor vitae</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>Amethyst Mckenzie</t>
+          <t>Dahlia Horn</t>
         </is>
       </c>
       <c r="B81" s="0" t="inlineStr">
         <is>
-          <t>(283) 556-0848</t>
+          <t>1-513-714-7485</t>
         </is>
       </c>
       <c r="C81" s="0" t="inlineStr">
         <is>
-          <t>nulla.ante@yahoo.org</t>
+          <t>ipsum.dolor@hotmail.org</t>
         </is>
       </c>
       <c r="D81" s="0" t="inlineStr">
         <is>
-          <t>Pará</t>
+          <t>Los Ríos</t>
         </is>
       </c>
       <c r="E81" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="F81" s="0" t="inlineStr">
         <is>
-          <t>at sem molestie sodales. Mauris blandit enim consequat purus. Maecenas</t>
+          <t>ipsum. Donec sollicitudin adipiscing ligula. Aenean gravida nunc sed pede.</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>Axel Butler</t>
+          <t>Orlando Donaldson</t>
         </is>
       </c>
       <c r="B82" s="0" t="inlineStr">
         <is>
-          <t>(314) 332-8526</t>
+          <t>1-855-754-7647</t>
         </is>
       </c>
       <c r="C82" s="0" t="inlineStr">
         <is>
-          <t>iaculis.aliquet.diam@protonmail.ca</t>
+          <t>tellus.aenean@icloud.edu</t>
         </is>
       </c>
       <c r="D82" s="0" t="inlineStr">
         <is>
-          <t>South Sumatra</t>
+          <t>Tasmania</t>
         </is>
       </c>
       <c r="E82" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="F82" s="0" t="inlineStr">
         <is>
-          <t>parturient montes, nascetur ridiculus mus. Proin vel arcu eu odio</t>
+          <t>elit elit fermentum risus, at fringilla purus mauris a nunc.</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>Mufutau Snow</t>
+          <t>Kylan Shelton</t>
         </is>
       </c>
       <c r="B83" s="0" t="inlineStr">
         <is>
-          <t>(614) 855-2064</t>
+          <t>(787) 788-3535</t>
         </is>
       </c>
       <c r="C83" s="0" t="inlineStr">
         <is>
-          <t>vitae.orci.phasellus@outlook.org</t>
+          <t>dictum.augue@protonmail.edu</t>
         </is>
       </c>
       <c r="D83" s="0" t="inlineStr">
         <is>
-          <t>Cartago</t>
+          <t>Antalya</t>
         </is>
       </c>
       <c r="E83" s="0" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F83" s="0" t="inlineStr">
         <is>
-          <t>nunc est, mollis non, cursus non, egestas a, dui. Cras</t>
+          <t>ligula. Aenean gravida nunc sed pede. Cum sociis natoque penatibus</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>Tana Campbell</t>
+          <t>Shana Tate</t>
         </is>
       </c>
       <c r="B84" s="0" t="inlineStr">
         <is>
-          <t>(244) 246-7211</t>
+          <t>1-483-363-3620</t>
         </is>
       </c>
       <c r="C84" s="0" t="inlineStr">
         <is>
-          <t>mollis.dui.in@outlook.org</t>
+          <t>suspendisse@icloud.net</t>
         </is>
       </c>
       <c r="D84" s="0" t="inlineStr">
         <is>
-          <t>Vlaams-Brabant</t>
+          <t>North Region</t>
         </is>
       </c>
       <c r="E84" s="0" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F84" s="0" t="inlineStr">
         <is>
-          <t>blandit enim consequat purus. Maecenas libero est, congue a, aliquet</t>
+          <t>arcu. Nunc mauris. Morbi non sapien molestie orci tincidunt adipiscing.</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>Cally Mclaughlin</t>
+          <t>Jesse Colon</t>
         </is>
       </c>
       <c r="B85" s="0" t="inlineStr">
         <is>
-          <t>(313) 315-1548</t>
+          <t>1-154-708-6487</t>
         </is>
       </c>
       <c r="C85" s="0" t="inlineStr">
         <is>
-          <t>erat.eget.ipsum@protonmail.edu</t>
+          <t>nec.diam.duis@outlook.org</t>
         </is>
       </c>
       <c r="D85" s="0" t="inlineStr">
         <is>
-          <t>Tarapacá</t>
+          <t>Limburg</t>
         </is>
       </c>
       <c r="E85" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F85" s="0" t="inlineStr">
         <is>
-          <t>augue eu tellus. Phasellus elit pede, malesuada vel, venenatis vel,</t>
+          <t>cursus. Integer mollis. Integer tincidunt aliquam arcu. Aliquam ultrices iaculis</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>Forrest Stevens</t>
+          <t>Kyla Gay</t>
         </is>
       </c>
       <c r="B86" s="0" t="inlineStr">
         <is>
-          <t>1-103-834-4584</t>
+          <t>1-814-435-4161</t>
         </is>
       </c>
       <c r="C86" s="0" t="inlineStr">
         <is>
-          <t>ultricies.adipiscing.enim@google.ca</t>
+          <t>donec.nibh@icloud.ca</t>
         </is>
       </c>
       <c r="D86" s="0" t="inlineStr">
         <is>
-          <t>Limburg</t>
+          <t>Nizhny Novgorod Oblast</t>
         </is>
       </c>
       <c r="E86" s="0" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="F86" s="0" t="inlineStr">
         <is>
-          <t>nec mauris blandit mattis. Cras eget nisi dictum augue malesuada</t>
+          <t>ac turpis egestas. Aliquam fringilla cursus purus. Nullam scelerisque neque</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>Caldwell Mullen</t>
+          <t>Cullen Singleton</t>
         </is>
       </c>
       <c r="B87" s="0" t="inlineStr">
         <is>
-          <t>(199) 977-3345</t>
+          <t>(324) 874-6756</t>
         </is>
       </c>
       <c r="C87" s="0" t="inlineStr">
         <is>
-          <t>vulputate@hotmail.edu</t>
+          <t>leo.in@hotmail.couk</t>
         </is>
       </c>
       <c r="D87" s="0" t="inlineStr">
         <is>
-          <t>Osun</t>
+          <t>Arica y Parinacota</t>
         </is>
       </c>
       <c r="E87" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="F87" s="0" t="inlineStr">
         <is>
-          <t>lacus. Quisque purus sapien, gravida non, sollicitudin a, malesuada id,</t>
+          <t>sit amet ante. Vivamus non lorem vitae odio sagittis semper.</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>Elvis Joyce</t>
+          <t>Zenia Cameron</t>
         </is>
       </c>
       <c r="B88" s="0" t="inlineStr">
         <is>
-          <t>(782) 897-7710</t>
+          <t>(982) 353-1632</t>
         </is>
       </c>
       <c r="C88" s="0" t="inlineStr">
         <is>
-          <t>facilisis.facilisis@icloud.org</t>
+          <t>facilisis@aol.com</t>
         </is>
       </c>
       <c r="D88" s="0" t="inlineStr">
         <is>
-          <t>South Island</t>
+          <t>Cajamarca</t>
         </is>
       </c>
       <c r="E88" s="0" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="F88" s="0" t="inlineStr">
         <is>
-          <t>in, dolor. Fusce feugiat. Lorem ipsum dolor sit amet, consectetuer</t>
+          <t>interdum ligula eu enim. Etiam imperdiet dictum magna. Ut tincidunt</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>Ryder Frazier</t>
+          <t>Amanda Gay</t>
         </is>
       </c>
       <c r="B89" s="0" t="inlineStr">
         <is>
-          <t>(767) 886-4710</t>
+          <t>1-444-795-0313</t>
         </is>
       </c>
       <c r="C89" s="0" t="inlineStr">
         <is>
-          <t>cursus.vestibulum@google.edu</t>
+          <t>sit.amet@outlook.couk</t>
         </is>
       </c>
       <c r="D89" s="0" t="inlineStr">
         <is>
-          <t>Vlaams-Brabant</t>
+          <t>Brandenburg</t>
         </is>
       </c>
       <c r="E89" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="F89" s="0" t="inlineStr">
         <is>
-          <t>lobortis risus. In mi pede, nonummy ut, molestie in, tempus</t>
+          <t>enim consequat purus. Maecenas libero est, congue a, aliquet vel,</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>Linus Farley</t>
+          <t>Cynthia Savage</t>
         </is>
       </c>
       <c r="B90" s="0" t="inlineStr">
         <is>
-          <t>1-731-616-1538</t>
+          <t>(168) 385-4454</t>
         </is>
       </c>
       <c r="C90" s="0" t="inlineStr">
         <is>
-          <t>vitae.sodales@hotmail.couk</t>
+          <t>diam.nunc.ullamcorper@yahoo.couk</t>
         </is>
       </c>
       <c r="D90" s="0" t="inlineStr">
         <is>
-          <t>National Capital Region</t>
+          <t>Zamboanga Peninsula</t>
         </is>
       </c>
       <c r="E90" s="0" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="F90" s="0" t="inlineStr">
         <is>
-          <t>a tortor. Nunc commodo auctor velit. Aliquam nisl. Nulla eu</t>
+          <t>dictum magna. Ut tincidunt orci quis lectus. Nullam suscipit, est</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>Flynn Bowman</t>
+          <t>Nina Sellers</t>
         </is>
       </c>
       <c r="B91" s="0" t="inlineStr">
         <is>
-          <t>1-430-438-9877</t>
+          <t>(380) 460-4786</t>
         </is>
       </c>
       <c r="C91" s="0" t="inlineStr">
         <is>
-          <t>tempor.erat.neque@aol.edu</t>
+          <t>sed.pede@hotmail.org</t>
         </is>
       </c>
       <c r="D91" s="0" t="inlineStr">
         <is>
-          <t>Osun</t>
+          <t>San Luis Potosí</t>
         </is>
       </c>
       <c r="E91" s="0" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="F91" s="0" t="inlineStr">
         <is>
-          <t>magnis dis parturient montes, nascetur ridiculus mus. Donec dignissim magna</t>
+          <t>urna justo faucibus lectus, a sollicitudin orci sem eget massa.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>Orla Preston</t>
+          <t>Levi Burch</t>
         </is>
       </c>
       <c r="B92" s="0" t="inlineStr">
         <is>
-          <t>(830) 473-6736</t>
+          <t>(578) 988-4883</t>
         </is>
       </c>
       <c r="C92" s="0" t="inlineStr">
         <is>
-          <t>luctus.aliquet.odio@hotmail.net</t>
+          <t>eu@hotmail.net</t>
         </is>
       </c>
       <c r="D92" s="0" t="inlineStr">
         <is>
-          <t>Kentucky</t>
+          <t>Limpopo</t>
         </is>
       </c>
       <c r="E92" s="0" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="F92" s="0" t="inlineStr">
         <is>
-          <t>Donec felis orci, adipiscing non, luctus sit amet, faucibus ut,</t>
+          <t>ultrices. Vivamus rhoncus. Donec est. Nunc ullamcorper, velit in aliquet</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>Martha Cochran</t>
+          <t>Charles Hess</t>
         </is>
       </c>
       <c r="B93" s="0" t="inlineStr">
         <is>
-          <t>1-373-542-6003</t>
+          <t>1-258-286-7816</t>
         </is>
       </c>
       <c r="C93" s="0" t="inlineStr">
         <is>
-          <t>elementum.sem@outlook.ca</t>
+          <t>risus.in.mi@outlook.com</t>
         </is>
       </c>
       <c r="D93" s="0" t="inlineStr">
         <is>
-          <t>Burgenland</t>
+          <t>Madrid</t>
         </is>
       </c>
       <c r="E93" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Vietnam</t>
         </is>
       </c>
       <c r="F93" s="0" t="inlineStr">
         <is>
-          <t>sagittis lobortis mauris. Suspendisse aliquet molestie tellus. Aenean egestas hendrerit</t>
+          <t>molestie tellus. Aenean egestas hendrerit neque. In ornare sagittis felis.</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>Jemima Rowland</t>
+          <t>Lydia Flowers</t>
         </is>
       </c>
       <c r="B94" s="0" t="inlineStr">
         <is>
-          <t>(397) 598-4214</t>
+          <t>1-277-377-5676</t>
         </is>
       </c>
       <c r="C94" s="0" t="inlineStr">
         <is>
-          <t>ullamcorper.duis.cursus@google.ca</t>
+          <t>quis@yahoo.ca</t>
         </is>
       </c>
       <c r="D94" s="0" t="inlineStr">
         <is>
-          <t>North Island</t>
+          <t>Gujarat</t>
         </is>
       </c>
       <c r="E94" s="0" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F94" s="0" t="inlineStr">
         <is>
-          <t>dui. Cum sociis natoque penatibus et magnis dis parturient montes,</t>
+          <t>placerat, augue. Sed molestie. Sed id risus quis diam luctus</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>Amery Roberts</t>
+          <t>Illana Nunez</t>
         </is>
       </c>
       <c r="B95" s="0" t="inlineStr">
         <is>
-          <t>(682) 858-9372</t>
+          <t>(769) 475-7664</t>
         </is>
       </c>
       <c r="C95" s="0" t="inlineStr">
         <is>
-          <t>augue.sed@yahoo.ca</t>
+          <t>sem.eget@protonmail.com</t>
         </is>
       </c>
       <c r="D95" s="0" t="inlineStr">
         <is>
-          <t>Overijssel</t>
+          <t>Junín</t>
         </is>
       </c>
       <c r="E95" s="0" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F95" s="0" t="inlineStr">
         <is>
-          <t>Quisque porttitor eros nec tellus. Nunc lectus pede, ultrices a,</t>
+          <t>lacus. Ut nec urna et arcu imperdiet ullamcorper. Duis at</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>Boris Kaufman</t>
+          <t>Ishmael Burgess</t>
         </is>
       </c>
       <c r="B96" s="0" t="inlineStr">
         <is>
-          <t>1-141-214-6738</t>
+          <t>1-473-866-4498</t>
         </is>
       </c>
       <c r="C96" s="0" t="inlineStr">
         <is>
-          <t>ligula.donec@aol.edu</t>
+          <t>ridiculus.mus@hotmail.net</t>
         </is>
       </c>
       <c r="D96" s="0" t="inlineStr">
         <is>
-          <t>Coahuila</t>
+          <t>Aragón</t>
         </is>
       </c>
       <c r="E96" s="0" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Peru</t>
         </is>
       </c>
       <c r="F96" s="0" t="inlineStr">
         <is>
-          <t>amet risus. Donec egestas. Aliquam nec enim. Nunc ut erat.</t>
+          <t>nulla. Integer urna. Vivamus molestie dapibus ligula. Aliquam erat volutpat.</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>Celeste Nicholson</t>
+          <t>Asher Cobb</t>
         </is>
       </c>
       <c r="B97" s="0" t="inlineStr">
         <is>
-          <t>1-568-556-4215</t>
+          <t>(913) 361-6683</t>
         </is>
       </c>
       <c r="C97" s="0" t="inlineStr">
         <is>
-          <t>consequat.enim@aol.com</t>
+          <t>eros.nam@icloud.ca</t>
         </is>
       </c>
       <c r="D97" s="0" t="inlineStr">
         <is>
-          <t>Styria</t>
+          <t>Omsk Oblast</t>
         </is>
       </c>
       <c r="E97" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="F97" s="0" t="inlineStr">
         <is>
-          <t>enim, gravida sit amet, dapibus id, blandit at, nisi. Cum</t>
+          <t>rutrum. Fusce dolor quam, elementum at, egestas a, scelerisque sed,</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>Vivien Morrison</t>
+          <t>Iris Diaz</t>
         </is>
       </c>
       <c r="B98" s="0" t="inlineStr">
         <is>
-          <t>(492) 883-4311</t>
+          <t>1-647-887-7863</t>
         </is>
       </c>
       <c r="C98" s="0" t="inlineStr">
         <is>
-          <t>metus.aliquam.erat@protonmail.com</t>
+          <t>elit@hotmail.ca</t>
         </is>
       </c>
       <c r="D98" s="0" t="inlineStr">
         <is>
-          <t>Saskatchewan</t>
+          <t>Connacht</t>
         </is>
       </c>
       <c r="E98" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F98" s="0" t="inlineStr">
         <is>
-          <t>ullamcorper, velit in aliquet lobortis, nisi nibh lacinia orci, consectetuer</t>
+          <t>mauris ut mi. Duis risus odio, auctor vitae, aliquet nec,</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>Freya Singleton</t>
+          <t>Calvin Barry</t>
         </is>
       </c>
       <c r="B99" s="0" t="inlineStr">
         <is>
-          <t>1-745-908-3836</t>
+          <t>1-271-938-4740</t>
         </is>
       </c>
       <c r="C99" s="0" t="inlineStr">
         <is>
-          <t>pharetra@hotmail.net</t>
+          <t>a@outlook.ca</t>
         </is>
       </c>
       <c r="D99" s="0" t="inlineStr">
         <is>
-          <t>Calabria</t>
+          <t>West Nusa Tenggara</t>
         </is>
       </c>
       <c r="E99" s="0" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F99" s="0" t="inlineStr">
         <is>
-          <t>Nullam suscipit, est ac facilisis facilisis, magna tellus faucibus leo,</t>
+          <t>elit fermentum risus, at fringilla purus mauris a nunc. In</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>Abraham Gibbs</t>
+          <t>Allegra Lowery</t>
         </is>
       </c>
       <c r="B100" s="0" t="inlineStr">
         <is>
-          <t>(213) 886-6430</t>
+          <t>(322) 390-8158</t>
         </is>
       </c>
       <c r="C100" s="0" t="inlineStr">
         <is>
-          <t>sagittis.augue.eu@hotmail.org</t>
+          <t>inceptos@outlook.edu</t>
         </is>
       </c>
       <c r="D100" s="0" t="inlineStr">
         <is>
-          <t>Styria</t>
+          <t>Eastern Cape</t>
         </is>
       </c>
       <c r="E100" s="0" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F100" s="0" t="inlineStr">
         <is>
-          <t>Vivamus euismod urna. Nullam lobortis quam a felis ullamcorper viverra.</t>
+          <t>Sed et libero. Proin mi. Aliquam gravida mauris ut mi.</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>Zane Davis</t>
+          <t>Yvonne Buckley</t>
         </is>
       </c>
       <c r="B101" s="0" t="inlineStr">
         <is>
-          <t>1-635-241-5966</t>
+          <t>1-762-730-6322</t>
         </is>
       </c>
       <c r="C101" s="0" t="inlineStr">
         <is>
-          <t>nullam.lobortis@yahoo.edu</t>
+          <t>odio.a@protonmail.ca</t>
         </is>
       </c>
       <c r="D101" s="0" t="inlineStr">
         <is>
-          <t>North Island</t>
+          <t>Friesland</t>
         </is>
       </c>
       <c r="E101" s="0" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F101" s="0" t="inlineStr">
         <is>
-          <t>eu augue porttitor interdum. Sed auctor odio a purus. Duis</t>
+          <t>ante ipsum primis in faucibus orci luctus et ultrices posuere</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
edit moulde table html and creat module export-csv export-xlsx
</commit_message>
<xml_diff>
--- a/crawler/publics/data.xlsx
+++ b/crawler/publics/data.xlsx
@@ -73,10 +73,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.18988764044944"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.28988764044944"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="15.18988764044944"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="28.389887640449437"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.18988764044944"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="27.28988764044944"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.48988764044944"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.18988764044944"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="59.18988764044944"/>
   </cols>
@@ -116,150 +116,150 @@
     <row r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>Petra Goff</t>
+          <t>Armand Wong</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>1-367-480-1708</t>
+          <t>(341) 330-4146</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>dictum.sapien.aenean@icloud.com</t>
+          <t>auctor.velit@icloud.org</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Agder</t>
+          <t>Khyber Pakhtoonkhwa</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>ultrices, mauris ipsum porta elit, a feugiat tellus lorem eu</t>
+          <t>Curabitur vel lectus. Cum sociis natoque penatibus et magnis dis</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>Alyssa Chandler</t>
+          <t>Ahmed Navarro</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
         <is>
-          <t>1-615-771-1021</t>
+          <t>(468) 311-6242</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>arcu.vestibulum@aol.couk</t>
+          <t>faucibus.morbi@icloud.org</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>Samsun</t>
+          <t>Odisha</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>metus urna convallis erat, eget tincidunt dui augue eu tellus.</t>
+          <t>eleifend egestas. Sed pharetra, felis eget varius ultrices, mauris ipsum</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>Adara Whitley</t>
+          <t>Zenia Noel</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>1-581-630-8134</t>
+          <t>1-514-410-7138</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>mauris.blandit.mattis@yahoo.couk</t>
+          <t>eu@google.org</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>North Jeolla</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>in consequat enim diam vel arcu. Curabitur ut odio vel</t>
+          <t>velit. Aliquam nisl. Nulla eu neque pellentesque massa lobortis ultrices.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>Aaron Thornton</t>
+          <t>Alexander Dixon</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>(116) 880-4806</t>
+          <t>1-428-864-6114</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>nullam.feugiat@yahoo.com</t>
+          <t>nam@google.edu</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>Kerala</t>
+          <t>Oslo</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>pede et risus. Quisque libero lacus, varius et, euismod et,</t>
+          <t>condimentum eget, volutpat ornare, facilisis eget, ipsum. Donec sollicitudin adipiscing</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>Camille Logan</t>
+          <t>Cecilia Sullivan</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
         <is>
-          <t>1-318-951-6726</t>
+          <t>(748) 722-0811</t>
         </is>
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>id.enim.curabitur@protonmail.ca</t>
+          <t>libero.est.congue@outlook.couk</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>Benue</t>
+          <t>Guanajuato</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
@@ -269,253 +269,253 @@
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>metus. In lorem. Donec elementum, lorem ut aliquam iaculis, lacus</t>
+          <t>ipsum dolor sit amet, consectetuer adipiscing elit. Aliquam auctor, velit</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>Kadeem Chang</t>
+          <t>Paula Kramer</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
         <is>
-          <t>1-247-380-5998</t>
+          <t>(619) 421-4018</t>
         </is>
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>dolor@outlook.ca</t>
+          <t>dui.cum@icloud.ca</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>Córdoba</t>
+          <t>Alberta</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>sapien, gravida non, sollicitudin a, malesuada id, erat. Etiam vestibulum</t>
+          <t>Curae Phasellus ornare. Fusce mollis. Duis sit amet diam eu</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>Brittany Manning</t>
+          <t>Brynne Mcbride</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
         <is>
-          <t>1-821-239-5556</t>
+          <t>1-508-343-3646</t>
         </is>
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>ad.litora@aol.edu</t>
+          <t>sed@protonmail.com</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>Warwickshire</t>
+          <t>Rio Grande do Sul</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>fringilla. Donec feugiat metus sit amet ante. Vivamus non lorem</t>
+          <t>placerat, orci lacus vestibulum lorem, sit amet ultricies sem magna</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>Nina English</t>
+          <t>Abdul Slater</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>1-995-947-4451</t>
+          <t>(441) 928-6684</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>interdum.libero@protonmail.net</t>
+          <t>et.magna@icloud.edu</t>
         </is>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>Puno</t>
+          <t>Zaporizhzhia oblast</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>sapien. Nunc pulvinar arcu et pede. Nunc sed orci lobortis</t>
+          <t>vitae, orci. Phasellus dapibus quam quis diam. Pellentesque habitant morbi</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>Jena Delaney</t>
+          <t>Silas Banks</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
         <is>
-          <t>(236) 831-7636</t>
+          <t>1-743-598-4274</t>
         </is>
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>cum.sociis@hotmail.net</t>
+          <t>tempus.non@icloud.com</t>
         </is>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>Bangsamoro</t>
+          <t>Azad Kashmir</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>magna. Lorem ipsum dolor sit amet, consectetuer adipiscing elit. Etiam</t>
+          <t>arcu. Curabitur ut odio vel est tempor bibendum. Donec felis</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>Inez Trevino</t>
+          <t>Luke Armstrong</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
         <is>
-          <t>(327) 137-3307</t>
+          <t>1-133-663-7077</t>
         </is>
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>sed@google.net</t>
+          <t>senectus.et.netus@aol.org</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>South Island</t>
+          <t>Katsina</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>Integer id magna et ipsum cursus vestibulum. Mauris magna. Duis</t>
+          <t>urna justo faucibus lectus, a sollicitudin orci sem eget massa.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>Hayfa Hampton</t>
+          <t>Gail Nolan</t>
         </is>
       </c>
       <c r="B12" s="0" t="inlineStr">
         <is>
-          <t>(761) 823-3825</t>
+          <t>1-305-375-4364</t>
         </is>
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>convallis@hotmail.couk</t>
+          <t>eu.euismod@aol.ca</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>Haute-Normandie</t>
+          <t>Jönköpings län</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>tincidunt adipiscing. Mauris molestie pharetra nibh. Aliquam ornare, libero at</t>
+          <t>penatibus et magnis dis parturient montes, nascetur ridiculus mus. Proin</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>Dai Kirby</t>
+          <t>Jade Chang</t>
         </is>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>(617) 839-7545</t>
+          <t>1-667-605-0184</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
         <is>
-          <t>erat.neque@hotmail.edu</t>
+          <t>ac.feugiat.non@protonmail.ca</t>
         </is>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>North Island</t>
+          <t>Ninh Thuận</t>
         </is>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>lectus rutrum urna, nec luctus felis purus ac tellus. Suspendisse</t>
+          <t>risus. Donec egestas. Duis ac arcu. Nunc mauris. Morbi non</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>Thane Hamilton</t>
+          <t>Ariana Barton</t>
         </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
         <is>
-          <t>(651) 155-5139</t>
+          <t>(724) 604-9839</t>
         </is>
       </c>
       <c r="C14" s="0" t="inlineStr">
         <is>
-          <t>eu.eros.nam@hotmail.ca</t>
+          <t>lorem.lorem@protonmail.couk</t>
         </is>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>New South Wales</t>
+          <t>Los Lagos</t>
         </is>
       </c>
       <c r="E14" s="0" t="inlineStr">
@@ -525,93 +525,93 @@
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>at pretium aliquet, metus urna convallis erat, eget tincidunt dui</t>
+          <t>enim mi tempor lorem, eget mollis lectus pede et risus.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>Reuben Mccoy</t>
+          <t>Charde Best</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
         <is>
-          <t>(826) 586-9725</t>
+          <t>1-816-280-1585</t>
         </is>
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>praesent@aol.com</t>
+          <t>tellus.lorem@protonmail.couk</t>
         </is>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>Brussels Hoofdstedelijk Gewest</t>
+          <t>Sachsen-Anhalt</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>non dui nec urna suscipit nonummy. Fusce fermentum fermentum arcu.</t>
+          <t>vehicula. Pellentesque tincidunt tempus risus. Donec egestas. Duis ac arcu.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>Gregory Pickett</t>
+          <t>Minerva Collier</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>(938) 675-4511</t>
+          <t>(781) 368-9723</t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
         <is>
-          <t>eu.enim@yahoo.com</t>
+          <t>in.lorem@google.couk</t>
         </is>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>Rivers</t>
+          <t>Australian Capital Territory</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>sagittis augue, eu tempor erat neque non quam. Pellentesque habitant</t>
+          <t>Donec est mauris, rhoncus id, mollis nec, cursus a, enim.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>Kyla Horn</t>
+          <t>Rhiannon Pope</t>
         </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
         <is>
-          <t>1-644-356-8496</t>
+          <t>(233) 814-2325</t>
         </is>
       </c>
       <c r="C17" s="0" t="inlineStr">
         <is>
-          <t>lacus.ut@protonmail.edu</t>
+          <t>nonummy@aol.edu</t>
         </is>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>Viken</t>
+          <t>North West</t>
         </is>
       </c>
       <c r="E17" s="0" t="inlineStr">
@@ -621,93 +621,93 @@
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>dictum sapien. Aenean massa. Integer vitae nibh. Donec est mauris,</t>
+          <t>turpis egestas. Aliquam fringilla cursus purus. Nullam scelerisque neque sed</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>Adrienne Santos</t>
+          <t>Carol Nixon</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
         <is>
-          <t>(742) 414-6856</t>
+          <t>1-710-280-8742</t>
         </is>
       </c>
       <c r="C18" s="0" t="inlineStr">
         <is>
-          <t>mauris.non.dui@google.com</t>
+          <t>commodo@aol.ca</t>
         </is>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>Ulyanovsk Oblast</t>
+          <t>Soccsksargen</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>sem, vitae aliquam eros turpis non enim. Mauris quis turpis</t>
+          <t>interdum enim non nisi. Aenean eget metus. In nec orci.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>Connor Willis</t>
+          <t>Raja Schroeder</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
         <is>
-          <t>1-615-901-8387</t>
+          <t>1-698-776-0288</t>
         </is>
       </c>
       <c r="C19" s="0" t="inlineStr">
         <is>
-          <t>sapien.cras.dolor@protonmail.edu</t>
+          <t>fringilla.ornare.placerat@google.ca</t>
         </is>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>Pembrokeshire</t>
+          <t>Sachsen</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>pretium et, rutrum non, hendrerit id, ante. Nunc mauris sapien,</t>
+          <t>sem ut cursus luctus, ipsum leo elementum sem, vitae aliquam</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>Alisa Oneil</t>
+          <t>Leah Odom</t>
         </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>1-362-623-4340</t>
+          <t>1-602-834-2389</t>
         </is>
       </c>
       <c r="C20" s="0" t="inlineStr">
         <is>
-          <t>ullamcorper@hotmail.couk</t>
+          <t>facilisis@aol.ca</t>
         </is>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>Opolskie</t>
+          <t>Leinster</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
@@ -717,189 +717,189 @@
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>amet, consectetuer adipiscing elit. Aliquam auctor, velit eget laoreet posuere,</t>
+          <t>commodo hendrerit. Donec porttitor tellus non magna. Nam ligula elit,</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>Malachi Velez</t>
+          <t>Howard Anthony</t>
         </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
         <is>
-          <t>1-830-746-2193</t>
+          <t>(341) 593-3291</t>
         </is>
       </c>
       <c r="C21" s="0" t="inlineStr">
         <is>
-          <t>lorem.ipsum@aol.net</t>
+          <t>faucibus@yahoo.couk</t>
         </is>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>Zeeland</t>
+          <t>Oslo</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t>a nunc. In at pede. Cras vulputate velit eu sem.</t>
+          <t>ligula elit, pretium et, rutrum non, hendrerit id, ante. Nunc</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>Ivana Best</t>
+          <t>Jayme Parks</t>
         </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
         <is>
-          <t>1-963-844-3676</t>
+          <t>1-833-787-5747</t>
         </is>
       </c>
       <c r="C22" s="0" t="inlineStr">
         <is>
-          <t>eget@aol.couk</t>
+          <t>a.ultricies.adipiscing@outlook.org</t>
         </is>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>Liguria</t>
+          <t>Manitoba</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t>Vivamus nibh dolor, nonummy ac, feugiat non, lobortis quis, pede.</t>
+          <t>Nam tempor diam dictum sapien. Aenean massa. Integer vitae nibh.</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>Breanna Morrow</t>
+          <t>Hu Richards</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>(571) 524-5134</t>
+          <t>(592) 632-3385</t>
         </is>
       </c>
       <c r="C23" s="0" t="inlineStr">
         <is>
-          <t>natoque@aol.org</t>
+          <t>nulla.dignissim@yahoo.com</t>
         </is>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>Tuyên Quang</t>
+          <t>Azad Kashmir</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>in, cursus et, eros. Proin ultrices. Duis volutpat nunc sit</t>
+          <t>ac tellus. Suspendisse sed dolor. Fusce mi lorem, vehicula et,</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>Salvador Whitaker</t>
+          <t>Sade Sullivan</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>1-146-335-5316</t>
+          <t>1-496-887-9318</t>
         </is>
       </c>
       <c r="C24" s="0" t="inlineStr">
         <is>
-          <t>tortor@google.couk</t>
+          <t>eget@aol.edu</t>
         </is>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>Campania</t>
+          <t>North Gyeongsang</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>ligula tortor, dictum eu, placerat eget, venenatis a, magna. Lorem</t>
+          <t>urna. Nunc quis arcu vel quam dignissim pharetra. Nam ac</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>Jared Holcomb</t>
+          <t>Isabella Wilder</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>(799) 207-3672</t>
+          <t>(624) 648-1062</t>
         </is>
       </c>
       <c r="C25" s="0" t="inlineStr">
         <is>
-          <t>nulla.at@icloud.couk</t>
+          <t>imperdiet.ullamcorper.duis@icloud.com</t>
         </is>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>Heredia</t>
+          <t>Gyeonggi</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>mollis vitae, posuere at, velit. Cras lorem lorem, luctus ut,</t>
+          <t>lacinia mattis. Integer eu lacus. Quisque imperdiet, erat nonummy ultricies</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>Claire Rhodes</t>
+          <t>Fredericka Gilliam</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>1-865-111-1747</t>
+          <t>(892) 721-1758</t>
         </is>
       </c>
       <c r="C26" s="0" t="inlineStr">
         <is>
-          <t>vel.sapien@aol.couk</t>
+          <t>in.hendrerit.consectetuer@aol.ca</t>
         </is>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>Schleswig-Holstein</t>
+          <t>North Region</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
@@ -909,1565 +909,1565 @@
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>consequat enim diam vel arcu. Curabitur ut odio vel est</t>
+          <t>eu eros. Nam consequat dolor vitae dolor. Donec fringilla. Donec</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>Aspen Robbins</t>
+          <t>Daquan Ruiz</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>(112) 964-6836</t>
+          <t>1-775-459-7054</t>
         </is>
       </c>
       <c r="C27" s="0" t="inlineStr">
         <is>
-          <t>scelerisque@outlook.edu</t>
+          <t>lorem.ut@yahoo.couk</t>
         </is>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>Morayshire</t>
+          <t>Puntarenas</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>augue porttitor interdum. Sed auctor odio a purus. Duis elementum,</t>
+          <t>enim, sit amet ornare lectus justo eu arcu. Morbi sit</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>Noel Hopkins</t>
+          <t>Seth Burke</t>
         </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>1-357-924-4337</t>
+          <t>1-480-864-4767</t>
         </is>
       </c>
       <c r="C28" s="0" t="inlineStr">
         <is>
-          <t>pede.nec@outlook.net</t>
+          <t>sem.pellentesque.ut@aol.ca</t>
         </is>
       </c>
       <c r="D28" s="0" t="inlineStr">
         <is>
-          <t>Waals-Brabant</t>
+          <t>Xīnán</t>
         </is>
       </c>
       <c r="E28" s="0" t="inlineStr">
         <is>
-          <t>Brazil</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F28" s="0" t="inlineStr">
         <is>
-          <t>Cras dictum ultricies ligula. Nullam enim. Sed nulla ante, iaculis</t>
+          <t>molestie. Sed id risus quis diam luctus lobortis. Class aptent</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>Naomi Berg</t>
+          <t>Aurelia Noel</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>1-877-595-3654</t>
+          <t>1-324-286-7335</t>
         </is>
       </c>
       <c r="C29" s="0" t="inlineStr">
         <is>
-          <t>elit@protonmail.edu</t>
+          <t>mi@google.edu</t>
         </is>
       </c>
       <c r="D29" s="0" t="inlineStr">
         <is>
-          <t>Murcia</t>
+          <t>Chiapas</t>
         </is>
       </c>
       <c r="E29" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F29" s="0" t="inlineStr">
         <is>
-          <t>Nunc pulvinar arcu et pede. Nunc sed orci lobortis augue</t>
+          <t>at fringilla purus mauris a nunc. In at pede. Cras</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>Nash Foreman</t>
+          <t>Rafael Marquez</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>1-244-825-5275</t>
+          <t>1-427-553-7369</t>
         </is>
       </c>
       <c r="C30" s="0" t="inlineStr">
         <is>
-          <t>dolor.dolor.tempus@yahoo.com</t>
+          <t>lorem.tristique@hotmail.edu</t>
         </is>
       </c>
       <c r="D30" s="0" t="inlineStr">
         <is>
-          <t>Şanlıurfa</t>
+          <t>Poltava oblast</t>
         </is>
       </c>
       <c r="E30" s="0" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Costa Rica</t>
         </is>
       </c>
       <c r="F30" s="0" t="inlineStr">
         <is>
-          <t>dolor. Fusce feugiat. Lorem ipsum dolor sit amet, consectetuer adipiscing</t>
+          <t>ultrices sit amet, risus. Donec nibh enim, gravida sit amet,</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>Avram Avila</t>
+          <t>Rachel Harris</t>
         </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>1-124-452-1437</t>
+          <t>1-815-425-7847</t>
         </is>
       </c>
       <c r="C31" s="0" t="inlineStr">
         <is>
-          <t>tincidunt.adipiscing.mauris@hotmail.edu</t>
+          <t>molestie@aol.ca</t>
         </is>
       </c>
       <c r="D31" s="0" t="inlineStr">
         <is>
-          <t>Jammu and Kashmir</t>
+          <t>Sonora</t>
         </is>
       </c>
       <c r="E31" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="F31" s="0" t="inlineStr">
         <is>
-          <t>in sodales elit erat vitae risus. Duis a mi fringilla</t>
+          <t>non sapien molestie orci tincidunt adipiscing. Mauris molestie pharetra nibh.</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>Courtney Griffith</t>
+          <t>Gary Forbes</t>
         </is>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>1-964-494-1347</t>
+          <t>(920) 855-2706</t>
         </is>
       </c>
       <c r="C32" s="0" t="inlineStr">
         <is>
-          <t>duis.gravida@yahoo.ca</t>
+          <t>nec.ligula.consectetuer@yahoo.ca</t>
         </is>
       </c>
       <c r="D32" s="0" t="inlineStr">
         <is>
-          <t>Maranhão</t>
+          <t>Cornwall</t>
         </is>
       </c>
       <c r="E32" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="F32" s="0" t="inlineStr">
         <is>
-          <t>tellus non magna. Nam ligula elit, pretium et, rutrum non,</t>
+          <t>enim diam vel arcu. Curabitur ut odio vel est tempor</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>Tashya Alston</t>
+          <t>Lesley Brewer</t>
         </is>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>1-318-313-8211</t>
+          <t>(401) 473-9821</t>
         </is>
       </c>
       <c r="C33" s="0" t="inlineStr">
         <is>
-          <t>varius.orci@google.org</t>
+          <t>tellus.sem@icloud.ca</t>
         </is>
       </c>
       <c r="D33" s="0" t="inlineStr">
         <is>
-          <t>Khyber Pakhtoonkhwa</t>
+          <t>Luik</t>
         </is>
       </c>
       <c r="E33" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F33" s="0" t="inlineStr">
         <is>
-          <t>vulputate dui, nec tempus mauris erat eget ipsum. Suspendisse sagittis.</t>
+          <t>a tortor. Nunc commodo auctor velit. Aliquam nisl. Nulla eu</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>Nigel Hodges</t>
+          <t>Marcia Sloan</t>
         </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>1-641-242-6044</t>
+          <t>(345) 484-3281</t>
         </is>
       </c>
       <c r="C34" s="0" t="inlineStr">
         <is>
-          <t>at.risus@protonmail.com</t>
+          <t>nulla@icloud.net</t>
         </is>
       </c>
       <c r="D34" s="0" t="inlineStr">
         <is>
-          <t>Flevoland</t>
+          <t>Jönköpings län</t>
         </is>
       </c>
       <c r="E34" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F34" s="0" t="inlineStr">
         <is>
-          <t>sed pede nec ante blandit viverra. Donec tempus, lorem fringilla</t>
+          <t>sit amet orci. Ut sagittis lobortis mauris. Suspendisse aliquet molestie</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>Echo Watkins</t>
+          <t>Jordan Mercado</t>
         </is>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>(433) 217-2128</t>
+          <t>1-653-765-0638</t>
         </is>
       </c>
       <c r="C35" s="0" t="inlineStr">
         <is>
-          <t>eu.nibh@hotmail.ca</t>
+          <t>lacus.quisque@yahoo.com</t>
         </is>
       </c>
       <c r="D35" s="0" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Đắk Lắk</t>
         </is>
       </c>
       <c r="E35" s="0" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="F35" s="0" t="inlineStr">
         <is>
-          <t>Etiam bibendum fermentum metus. Aenean sed pede nec ante blandit</t>
+          <t>tempus risus. Donec egestas. Duis ac arcu. Nunc mauris. Morbi</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>Jana Woods</t>
+          <t>Jamalia Burt</t>
         </is>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>1-323-483-7567</t>
+          <t>(761) 696-6188</t>
         </is>
       </c>
       <c r="C36" s="0" t="inlineStr">
         <is>
-          <t>dapibus@icloud.couk</t>
+          <t>eu.erat@yahoo.ca</t>
         </is>
       </c>
       <c r="D36" s="0" t="inlineStr">
         <is>
-          <t>Huádōng</t>
+          <t>Ontario</t>
         </is>
       </c>
       <c r="E36" s="0" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F36" s="0" t="inlineStr">
         <is>
-          <t>natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus.</t>
+          <t>Nunc pulvinar arcu et pede. Nunc sed orci lobortis augue</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>Hop Frye</t>
+          <t>Branden Maldonado</t>
         </is>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>1-953-464-7173</t>
+          <t>(233) 417-8191</t>
         </is>
       </c>
       <c r="C37" s="0" t="inlineStr">
         <is>
-          <t>gravida.mauris@hotmail.com</t>
+          <t>nulla.cras.eu@google.ca</t>
         </is>
       </c>
       <c r="D37" s="0" t="inlineStr">
         <is>
-          <t>Viken</t>
+          <t>Drenthe</t>
         </is>
       </c>
       <c r="E37" s="0" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="F37" s="0" t="inlineStr">
         <is>
-          <t>Nunc ullamcorper, velit in aliquet lobortis, nisi nibh lacinia orci,</t>
+          <t>dui nec urna suscipit nonummy. Fusce fermentum fermentum arcu. Vestibulum</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>Carissa Slater</t>
+          <t>Hasad Conrad</t>
         </is>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>1-782-360-2678</t>
+          <t>1-732-502-3778</t>
         </is>
       </c>
       <c r="C38" s="0" t="inlineStr">
         <is>
-          <t>nulla.integer.urna@yahoo.net</t>
+          <t>morbi.vehicula@outlook.com</t>
         </is>
       </c>
       <c r="D38" s="0" t="inlineStr">
         <is>
-          <t>Upper Austria</t>
+          <t>łódzkie</t>
         </is>
       </c>
       <c r="E38" s="0" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F38" s="0" t="inlineStr">
         <is>
-          <t>tellus eu augue porttitor interdum. Sed auctor odio a purus.</t>
+          <t>elit. Aliquam auctor, velit eget laoreet posuere, enim nisl elementum</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>Rachel Meyers</t>
+          <t>Myra Sloan</t>
         </is>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>(764) 535-8528</t>
+          <t>(259) 758-9731</t>
         </is>
       </c>
       <c r="C39" s="0" t="inlineStr">
         <is>
-          <t>eleifend@yahoo.org</t>
+          <t>dapibus@yahoo.org</t>
         </is>
       </c>
       <c r="D39" s="0" t="inlineStr">
         <is>
-          <t>Sinaloa</t>
+          <t>Lubuskie</t>
         </is>
       </c>
       <c r="E39" s="0" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="F39" s="0" t="inlineStr">
         <is>
-          <t>tellus sem mollis dui, in sodales elit erat vitae risus.</t>
+          <t>fringilla, porttitor vulputate, posuere vulputate, lacus. Cras interdum. Nunc sollicitudin</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>Audrey Page</t>
+          <t>Shana Holloway</t>
         </is>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>(699) 822-8596</t>
+          <t>1-281-585-1613</t>
         </is>
       </c>
       <c r="C40" s="0" t="inlineStr">
         <is>
-          <t>nec.ligula@protonmail.net</t>
+          <t>euismod.est@google.net</t>
         </is>
       </c>
       <c r="D40" s="0" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>National Capital Region</t>
         </is>
       </c>
       <c r="E40" s="0" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F40" s="0" t="inlineStr">
         <is>
-          <t>hendrerit. Donec porttitor tellus non magna. Nam ligula elit, pretium</t>
+          <t>arcu. Vestibulum ut eros non enim commodo hendrerit. Donec porttitor</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>Carlos Knight</t>
+          <t>Julie Orr</t>
         </is>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>1-549-374-4834</t>
+          <t>(521) 334-3746</t>
         </is>
       </c>
       <c r="C41" s="0" t="inlineStr">
         <is>
-          <t>duis@yahoo.org</t>
+          <t>pellentesque.habitant@google.net</t>
         </is>
       </c>
       <c r="D41" s="0" t="inlineStr">
         <is>
-          <t>Styria</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="E41" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F41" s="0" t="inlineStr">
         <is>
-          <t>lorem, eget mollis lectus pede et risus. Quisque libero lacus,</t>
+          <t>sed pede nec ante blandit viverra. Donec tempus, lorem fringilla</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>Aurelia Hull</t>
+          <t>Benedict Dalton</t>
         </is>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>1-460-798-7577</t>
+          <t>(530) 853-6149</t>
         </is>
       </c>
       <c r="C42" s="0" t="inlineStr">
         <is>
-          <t>etiam.gravida@yahoo.com</t>
+          <t>eros.nam@aol.couk</t>
         </is>
       </c>
       <c r="D42" s="0" t="inlineStr">
         <is>
-          <t>Friuli-Venezia Giulia</t>
+          <t>Punjab</t>
         </is>
       </c>
       <c r="E42" s="0" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F42" s="0" t="inlineStr">
         <is>
-          <t>lectus, a sollicitudin orci sem eget massa. Suspendisse eleifend. Cras</t>
+          <t>convallis, ante lectus convallis est, vitae sodales nisi magna sed</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>Eugenia Fitzgerald</t>
+          <t>Abigail Montgomery</t>
         </is>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>1-662-608-7648</t>
+          <t>1-824-525-4888</t>
         </is>
       </c>
       <c r="C43" s="0" t="inlineStr">
         <is>
-          <t>ullamcorper@outlook.ca</t>
+          <t>elit.fermentum@icloud.com</t>
         </is>
       </c>
       <c r="D43" s="0" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>Lazio</t>
         </is>
       </c>
       <c r="E43" s="0" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F43" s="0" t="inlineStr">
         <is>
-          <t>mi lorem, vehicula et, rutrum eu, ultrices sit amet, risus.</t>
+          <t>Duis gravida. Praesent eu nulla at sem molestie sodales. Mauris</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>Geoffrey Sherman</t>
+          <t>Serina Merritt</t>
         </is>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>1-281-263-9907</t>
+          <t>1-352-112-4475</t>
         </is>
       </c>
       <c r="C44" s="0" t="inlineStr">
         <is>
-          <t>nonummy.ipsum@yahoo.ca</t>
+          <t>hendrerit.a@outlook.ca</t>
         </is>
       </c>
       <c r="D44" s="0" t="inlineStr">
         <is>
-          <t>Antofagasta</t>
+          <t>Western Australia</t>
         </is>
       </c>
       <c r="E44" s="0" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F44" s="0" t="inlineStr">
         <is>
-          <t>risus. Nunc ac sem ut dolor dapibus gravida. Aliquam tincidunt,</t>
+          <t>vitae, sodales at, velit. Pellentesque ultricies dignissim lacus. Aliquam rutrum</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>Tanner Barber</t>
+          <t>Kyle Stevenson</t>
         </is>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>1-706-323-3846</t>
+          <t>1-855-918-3546</t>
         </is>
       </c>
       <c r="C45" s="0" t="inlineStr">
         <is>
-          <t>risus.quis@outlook.net</t>
+          <t>vestibulum.accumsan.neque@yahoo.edu</t>
         </is>
       </c>
       <c r="D45" s="0" t="inlineStr">
         <is>
-          <t>Namen</t>
+          <t>Puntarenas</t>
         </is>
       </c>
       <c r="E45" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F45" s="0" t="inlineStr">
         <is>
-          <t>Integer sem elit, pharetra ut, pharetra sed, hendrerit a, arcu.</t>
+          <t>id, erat. Etiam vestibulum massa rutrum magna. Cras convallis convallis</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>Rahim Huber</t>
+          <t>Tamara Mack</t>
         </is>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>1-841-641-1266</t>
+          <t>1-333-685-9425</t>
         </is>
       </c>
       <c r="C46" s="0" t="inlineStr">
         <is>
-          <t>gravida.praesent.eu@protonmail.com</t>
+          <t>libero.morbi@yahoo.net</t>
         </is>
       </c>
       <c r="D46" s="0" t="inlineStr">
         <is>
-          <t>Zuid Holland</t>
+          <t>Northern Cape</t>
         </is>
       </c>
       <c r="E46" s="0" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="F46" s="0" t="inlineStr">
         <is>
-          <t>egestas. Aliquam fringilla cursus purus. Nullam scelerisque neque sed sem</t>
+          <t>orci luctus et ultrices posuere cubilia Curae Donec tincidunt. Donec</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>Rina Massey</t>
+          <t>Patrick Schneider</t>
         </is>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>1-578-315-5891</t>
+          <t>(833) 696-3855</t>
         </is>
       </c>
       <c r="C47" s="0" t="inlineStr">
         <is>
-          <t>iaculis.aliquet.diam@google.com</t>
+          <t>rutrum@outlook.edu</t>
         </is>
       </c>
       <c r="D47" s="0" t="inlineStr">
         <is>
-          <t>Małopolskie</t>
+          <t>Jalisco</t>
         </is>
       </c>
       <c r="E47" s="0" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Chile</t>
         </is>
       </c>
       <c r="F47" s="0" t="inlineStr">
         <is>
-          <t>vel, convallis in, cursus et, eros. Proin ultrices. Duis volutpat</t>
+          <t>massa. Quisque porttitor eros nec tellus. Nunc lectus pede, ultrices</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>Branden Hanson</t>
+          <t>Lee Levine</t>
         </is>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>1-435-872-0877</t>
+          <t>(810) 168-6673</t>
         </is>
       </c>
       <c r="C48" s="0" t="inlineStr">
         <is>
-          <t>ridiculus@yahoo.ca</t>
+          <t>ac.arcu@yahoo.org</t>
         </is>
       </c>
       <c r="D48" s="0" t="inlineStr">
         <is>
-          <t>São Paulo</t>
+          <t>Emilia-Romagna</t>
         </is>
       </c>
       <c r="E48" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F48" s="0" t="inlineStr">
         <is>
-          <t>augue. Sed molestie. Sed id risus quis diam luctus lobortis.</t>
+          <t>euismod enim. Etiam gravida molestie arcu. Sed eu nibh vulputate</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>Chava Jennings</t>
+          <t>Hope Porter</t>
         </is>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>1-892-754-0688</t>
+          <t>1-261-450-4286</t>
         </is>
       </c>
       <c r="C49" s="0" t="inlineStr">
         <is>
-          <t>consequat.nec@aol.edu</t>
+          <t>fusce.fermentum@google.net</t>
         </is>
       </c>
       <c r="D49" s="0" t="inlineStr">
         <is>
-          <t>Jigawa</t>
+          <t>Azad Kashmir</t>
         </is>
       </c>
       <c r="E49" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Pakistan</t>
         </is>
       </c>
       <c r="F49" s="0" t="inlineStr">
         <is>
-          <t>malesuada malesuada. Integer id magna et ipsum cursus vestibulum. Mauris</t>
+          <t>In nec orci. Donec nibh. Quisque nonummy ipsum non arcu.</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>Carissa Stewart</t>
+          <t>Brady Bird</t>
         </is>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>(313) 134-2198</t>
+          <t>(342) 615-9530</t>
         </is>
       </c>
       <c r="C50" s="0" t="inlineStr">
         <is>
-          <t>at.arcu@google.org</t>
+          <t>cum@icloud.ca</t>
         </is>
       </c>
       <c r="D50" s="0" t="inlineStr">
         <is>
-          <t>Vorarlberg</t>
+          <t>Sokoto</t>
         </is>
       </c>
       <c r="E50" s="0" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F50" s="0" t="inlineStr">
         <is>
-          <t>libero. Proin sed turpis nec mauris blandit mattis. Cras eget</t>
+          <t>volutpat. Nulla dignissim. Maecenas ornare egestas ligula. Nullam feugiat placerat</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>Dexter Suarez</t>
+          <t>Mari Wilcox</t>
         </is>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>1-446-863-4381</t>
+          <t>1-885-294-4685</t>
         </is>
       </c>
       <c r="C51" s="0" t="inlineStr">
         <is>
-          <t>nibh.aliquam.ornare@aol.couk</t>
+          <t>nibh.lacinia.orci@protonmail.couk</t>
         </is>
       </c>
       <c r="D51" s="0" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Jönköpings län</t>
         </is>
       </c>
       <c r="E51" s="0" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="F51" s="0" t="inlineStr">
         <is>
-          <t>Cras dolor dolor, tempus non, lacinia at, iaculis quis, pede.</t>
+          <t>mi lacinia mattis. Integer eu lacus. Quisque imperdiet, erat nonummy</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>Marshall Carrillo</t>
+          <t>Neville Strong</t>
         </is>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>1-445-476-9220</t>
+          <t>1-886-488-7857</t>
         </is>
       </c>
       <c r="C52" s="0" t="inlineStr">
         <is>
-          <t>lacinia@protonmail.com</t>
+          <t>volutpat.ornare.facilisis@outlook.ca</t>
         </is>
       </c>
       <c r="D52" s="0" t="inlineStr">
         <is>
-          <t>Mexico City</t>
+          <t>Ancash</t>
         </is>
       </c>
       <c r="E52" s="0" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F52" s="0" t="inlineStr">
         <is>
-          <t>velit justo nec ante. Maecenas mi felis, adipiscing fringilla, porttitor</t>
+          <t>et magnis dis parturient montes, nascetur ridiculus mus. Donec dignissim</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>Jameson Glass</t>
+          <t>Kiayada Norris</t>
         </is>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
-          <t>1-721-569-5615</t>
+          <t>(187) 323-4156</t>
         </is>
       </c>
       <c r="C53" s="0" t="inlineStr">
         <is>
-          <t>commodo.hendrerit@aol.net</t>
+          <t>faucibus.orci@aol.net</t>
         </is>
       </c>
       <c r="D53" s="0" t="inlineStr">
         <is>
-          <t>Tyrol</t>
+          <t>Ulyanovsk Oblast</t>
         </is>
       </c>
       <c r="E53" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F53" s="0" t="inlineStr">
         <is>
-          <t>eget magna. Suspendisse tristique neque venenatis lacus. Etiam bibendum fermentum</t>
+          <t>magna. Sed eu eros. Nam consequat dolor vitae dolor. Donec</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>Yuli Jennings</t>
+          <t>Luke Sweet</t>
         </is>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>1-476-418-7568</t>
+          <t>(546) 271-6113</t>
         </is>
       </c>
       <c r="C54" s="0" t="inlineStr">
         <is>
-          <t>molestie.arcu.sed@aol.com</t>
+          <t>blandit.enim.consequat@outlook.couk</t>
         </is>
       </c>
       <c r="D54" s="0" t="inlineStr">
         <is>
-          <t>Limburg</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="E54" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F54" s="0" t="inlineStr">
         <is>
-          <t>augue ac ipsum. Phasellus vitae mauris sit amet lorem semper</t>
+          <t>ac urna. Ut tincidunt vehicula risus. Nulla eget metus eu</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>Heidi Good</t>
+          <t>Maile Kane</t>
         </is>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>1-335-430-5385</t>
+          <t>1-674-784-4445</t>
         </is>
       </c>
       <c r="C55" s="0" t="inlineStr">
         <is>
-          <t>nulla.eget@icloud.net</t>
+          <t>nisi.magna@aol.edu</t>
         </is>
       </c>
       <c r="D55" s="0" t="inlineStr">
         <is>
-          <t>Western Australia</t>
+          <t>Chiapas</t>
         </is>
       </c>
       <c r="E55" s="0" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="F55" s="0" t="inlineStr">
         <is>
-          <t>magna nec quam. Curabitur vel lectus. Cum sociis natoque penatibus</t>
+          <t>nonummy ipsum non arcu. Vivamus sit amet risus. Donec egestas.</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>Jackson Walsh</t>
+          <t>Sara Cortez</t>
         </is>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
-          <t>(643) 861-8241</t>
+          <t>1-743-963-1540</t>
         </is>
       </c>
       <c r="C56" s="0" t="inlineStr">
         <is>
-          <t>pharetra@hotmail.couk</t>
+          <t>donec@outlook.net</t>
         </is>
       </c>
       <c r="D56" s="0" t="inlineStr">
         <is>
-          <t>Xīnán</t>
+          <t>Vienna</t>
         </is>
       </c>
       <c r="E56" s="0" t="inlineStr">
         <is>
-          <t>Chile</t>
+          <t>New Zealand</t>
         </is>
       </c>
       <c r="F56" s="0" t="inlineStr">
         <is>
-          <t>Duis dignissim tempor arcu. Vestibulum ut eros non enim commodo</t>
+          <t>ornare, elit elit fermentum risus, at fringilla purus mauris a</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>Rhea Bryan</t>
+          <t>Zane Joyner</t>
         </is>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
-          <t>1-106-445-4638</t>
+          <t>(982) 888-7855</t>
         </is>
       </c>
       <c r="C57" s="0" t="inlineStr">
         <is>
-          <t>amet.faucibus.ut@hotmail.net</t>
+          <t>hendrerit@icloud.couk</t>
         </is>
       </c>
       <c r="D57" s="0" t="inlineStr">
         <is>
-          <t>Kogi</t>
+          <t>Chernivtsi oblast</t>
         </is>
       </c>
       <c r="E57" s="0" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F57" s="0" t="inlineStr">
         <is>
-          <t>diam nunc, ullamcorper eu, euismod ac, fermentum vel, mauris. Integer</t>
+          <t>dis parturient montes, nascetur ridiculus mus. Donec dignissim magna a</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>Sarah Garcia</t>
+          <t>Regina Hicks</t>
         </is>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
-          <t>1-412-471-4014</t>
+          <t>1-546-595-2547</t>
         </is>
       </c>
       <c r="C58" s="0" t="inlineStr">
         <is>
-          <t>curabitur@hotmail.org</t>
+          <t>vulputate.lacus@icloud.org</t>
         </is>
       </c>
       <c r="D58" s="0" t="inlineStr">
         <is>
-          <t>Mecklenburg-Vorpommern</t>
+          <t>Île-de-France</t>
         </is>
       </c>
       <c r="E58" s="0" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F58" s="0" t="inlineStr">
         <is>
-          <t>lacinia at, iaculis quis, pede. Praesent eu dui. Cum sociis</t>
+          <t>consectetuer rhoncus. Nullam velit dui, semper et, lacinia vitae, sodales</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>Mallory Hunter</t>
+          <t>Jamalia Molina</t>
         </is>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
-          <t>1-652-411-5782</t>
+          <t>1-813-505-3652</t>
         </is>
       </c>
       <c r="C59" s="0" t="inlineStr">
         <is>
-          <t>litora.torquent@outlook.edu</t>
+          <t>lorem@outlook.edu</t>
         </is>
       </c>
       <c r="D59" s="0" t="inlineStr">
         <is>
-          <t>Rivne oblast</t>
+          <t>South Kalimantan</t>
         </is>
       </c>
       <c r="E59" s="0" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F59" s="0" t="inlineStr">
         <is>
-          <t>ac turpis egestas. Fusce aliquet magna a neque. Nullam ut</t>
+          <t>natoque penatibus et magnis dis parturient montes, nascetur ridiculus mus.</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>Xyla Walton</t>
+          <t>Melyssa Dodson</t>
         </is>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
-          <t>1-854-229-1260</t>
+          <t>(886) 264-1942</t>
         </is>
       </c>
       <c r="C60" s="0" t="inlineStr">
         <is>
-          <t>aliquam.eu@protonmail.edu</t>
+          <t>mus.aenean.eget@yahoo.net</t>
         </is>
       </c>
       <c r="D60" s="0" t="inlineStr">
         <is>
-          <t>British Columbia</t>
+          <t>KwaZulu-Natal</t>
         </is>
       </c>
       <c r="E60" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F60" s="0" t="inlineStr">
         <is>
-          <t>nisi magna sed dui. Fusce aliquam, enim nec tempus scelerisque,</t>
+          <t>vitae diam. Proin dolor. Nulla semper tellus id nunc interdum</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>Cleo Chen</t>
+          <t>Alika Mcintyre</t>
         </is>
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
-          <t>(753) 487-4184</t>
+          <t>1-265-624-4814</t>
         </is>
       </c>
       <c r="C61" s="0" t="inlineStr">
         <is>
-          <t>libero.et@yahoo.ca</t>
+          <t>dui@outlook.couk</t>
         </is>
       </c>
       <c r="D61" s="0" t="inlineStr">
         <is>
-          <t>Västra Götalands län</t>
+          <t>Aragón</t>
         </is>
       </c>
       <c r="E61" s="0" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="F61" s="0" t="inlineStr">
         <is>
-          <t>ac mattis ornare, lectus ante dictum mi, ac mattis velit</t>
+          <t>nulla. Cras eu tellus eu augue porttitor interdum. Sed auctor</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>Ulric Davidson</t>
+          <t>Amal Gardner</t>
         </is>
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
-          <t>(669) 771-3826</t>
+          <t>(617) 713-2864</t>
         </is>
       </c>
       <c r="C62" s="0" t="inlineStr">
         <is>
-          <t>donec.nibh@hotmail.couk</t>
+          <t>aptent.taciti.sociosqu@protonmail.ca</t>
         </is>
       </c>
       <c r="D62" s="0" t="inlineStr">
         <is>
-          <t>Tabasco</t>
+          <t>Devon</t>
         </is>
       </c>
       <c r="E62" s="0" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>India</t>
         </is>
       </c>
       <c r="F62" s="0" t="inlineStr">
         <is>
-          <t>dictum sapien. Aenean massa. Integer vitae nibh. Donec est mauris,</t>
+          <t>pede. Cras vulputate velit eu sem. Pellentesque ut ipsum ac</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>Hayes Evans</t>
+          <t>Aquila Burt</t>
         </is>
       </c>
       <c r="B63" s="0" t="inlineStr">
         <is>
-          <t>1-807-694-2452</t>
+          <t>(623) 199-7841</t>
         </is>
       </c>
       <c r="C63" s="0" t="inlineStr">
         <is>
-          <t>cursus.integer@google.couk</t>
+          <t>nec.imperdiet.nec@icloud.edu</t>
         </is>
       </c>
       <c r="D63" s="0" t="inlineStr">
         <is>
-          <t>Schleswig-Holstein</t>
+          <t>Guanacaste</t>
         </is>
       </c>
       <c r="E63" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F63" s="0" t="inlineStr">
         <is>
-          <t>elit. Nulla facilisi. Sed neque. Sed eget lacus. Mauris non</t>
+          <t>odio vel est tempor bibendum. Donec felis orci, adipiscing non,</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>Ariel Hendricks</t>
+          <t>Pascale Hooper</t>
         </is>
       </c>
       <c r="B64" s="0" t="inlineStr">
         <is>
-          <t>(988) 771-4697</t>
+          <t>(604) 216-7757</t>
         </is>
       </c>
       <c r="C64" s="0" t="inlineStr">
         <is>
-          <t>tristique.senectus@yahoo.org</t>
+          <t>sociis@protonmail.org</t>
         </is>
       </c>
       <c r="D64" s="0" t="inlineStr">
         <is>
-          <t>Northern Cape</t>
+          <t>Jalisco</t>
         </is>
       </c>
       <c r="E64" s="0" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="F64" s="0" t="inlineStr">
         <is>
-          <t>penatibus et magnis dis parturient montes, nascetur ridiculus mus. Proin</t>
+          <t>blandit. Nam nulla magna, malesuada vel, convallis in, cursus et,</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>Irma Becker</t>
+          <t>Gary Richards</t>
         </is>
       </c>
       <c r="B65" s="0" t="inlineStr">
         <is>
-          <t>1-377-149-1673</t>
+          <t>(473) 196-3043</t>
         </is>
       </c>
       <c r="C65" s="0" t="inlineStr">
         <is>
-          <t>tempus.eu.ligula@google.edu</t>
+          <t>mollis.vitae.posuere@aol.couk</t>
         </is>
       </c>
       <c r="D65" s="0" t="inlineStr">
         <is>
-          <t>Chocó</t>
+          <t>Sucre</t>
         </is>
       </c>
       <c r="E65" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="F65" s="0" t="inlineStr">
         <is>
-          <t>Cras eget nisi dictum augue malesuada malesuada. Integer id magna</t>
+          <t>mi pede, nonummy ut, molestie in, tempus eu, ligula. Aenean</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>Lara Cross</t>
+          <t>Elliott Harrington</t>
         </is>
       </c>
       <c r="B66" s="0" t="inlineStr">
         <is>
-          <t>1-572-726-2481</t>
+          <t>(350) 860-8774</t>
         </is>
       </c>
       <c r="C66" s="0" t="inlineStr">
         <is>
-          <t>scelerisque.mollis@yahoo.org</t>
+          <t>lorem.ipsum@yahoo.org</t>
         </is>
       </c>
       <c r="D66" s="0" t="inlineStr">
         <is>
-          <t>Tula Oblast</t>
+          <t>Centre</t>
         </is>
       </c>
       <c r="E66" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="F66" s="0" t="inlineStr">
         <is>
-          <t>magna et ipsum cursus vestibulum. Mauris magna. Duis dignissim tempor</t>
+          <t>ac turpis egestas. Aliquam fringilla cursus purus. Nullam scelerisque neque</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>Mufutau Greer</t>
+          <t>Yasir Wall</t>
         </is>
       </c>
       <c r="B67" s="0" t="inlineStr">
         <is>
-          <t>1-588-748-5168</t>
+          <t>(926) 239-1841</t>
         </is>
       </c>
       <c r="C67" s="0" t="inlineStr">
         <is>
-          <t>fringilla.est@yahoo.org</t>
+          <t>duis.risus@icloud.com</t>
         </is>
       </c>
       <c r="D67" s="0" t="inlineStr">
         <is>
-          <t>North Sumatra</t>
+          <t>Xīnán</t>
         </is>
       </c>
       <c r="E67" s="0" t="inlineStr">
         <is>
-          <t>Pakistan</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F67" s="0" t="inlineStr">
         <is>
-          <t>adipiscing. Mauris molestie pharetra nibh. Aliquam ornare, libero at auctor</t>
+          <t>netus et malesuada fames ac turpis egestas. Aliquam fringilla cursus</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>Kameko Foster</t>
+          <t>Hashim Watkins</t>
         </is>
       </c>
       <c r="B68" s="0" t="inlineStr">
         <is>
-          <t>1-672-844-0763</t>
+          <t>(692) 752-6134</t>
         </is>
       </c>
       <c r="C68" s="0" t="inlineStr">
         <is>
-          <t>duis.risus@outlook.ca</t>
+          <t>dui.cum@google.couk</t>
         </is>
       </c>
       <c r="D68" s="0" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Chiapas</t>
         </is>
       </c>
       <c r="E68" s="0" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F68" s="0" t="inlineStr">
         <is>
-          <t>id nunc interdum feugiat. Sed nec metus facilisis lorem tristique</t>
+          <t>hymenaeos. Mauris ut quam vel sapien imperdiet ornare. In faucibus.</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>Jana Lamb</t>
+          <t>Dawn Franks</t>
         </is>
       </c>
       <c r="B69" s="0" t="inlineStr">
         <is>
-          <t>1-627-658-2668</t>
+          <t>1-216-498-2793</t>
         </is>
       </c>
       <c r="C69" s="0" t="inlineStr">
         <is>
-          <t>non.bibendum.sed@yahoo.com</t>
+          <t>ante@hotmail.org</t>
         </is>
       </c>
       <c r="D69" s="0" t="inlineStr">
         <is>
-          <t>Bình Định</t>
+          <t>North Sumatra</t>
         </is>
       </c>
       <c r="E69" s="0" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F69" s="0" t="inlineStr">
         <is>
-          <t>tristique senectus et netus et malesuada fames ac turpis egestas.</t>
+          <t>adipiscing. Mauris molestie pharetra nibh. Aliquam ornare, libero at auctor</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>David Watts</t>
+          <t>Amena Castillo</t>
         </is>
       </c>
       <c r="B70" s="0" t="inlineStr">
         <is>
-          <t>1-551-263-8428</t>
+          <t>1-441-269-4139</t>
         </is>
       </c>
       <c r="C70" s="0" t="inlineStr">
         <is>
-          <t>quis.turpis@icloud.ca</t>
+          <t>eu.eros.nam@icloud.org</t>
         </is>
       </c>
       <c r="D70" s="0" t="inlineStr">
         <is>
-          <t>Magadan Oblast</t>
+          <t>Connacht</t>
         </is>
       </c>
       <c r="E70" s="0" t="inlineStr">
         <is>
-          <t>Singapore</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="F70" s="0" t="inlineStr">
         <is>
-          <t>egestas hendrerit neque. In ornare sagittis felis. Donec tempor, est</t>
+          <t>arcu vel quam dignissim pharetra. Nam ac nulla. In tincidunt</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>Whitney Forbes</t>
+          <t>Adrian Lane</t>
         </is>
       </c>
       <c r="B71" s="0" t="inlineStr">
         <is>
-          <t>1-807-564-5527</t>
+          <t>(915) 900-4405</t>
         </is>
       </c>
       <c r="C71" s="0" t="inlineStr">
         <is>
-          <t>maecenas.mi@google.couk</t>
+          <t>nisl@protonmail.com</t>
         </is>
       </c>
       <c r="D71" s="0" t="inlineStr">
         <is>
-          <t>FATA</t>
+          <t>Haute-Normandie</t>
         </is>
       </c>
       <c r="E71" s="0" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F71" s="0" t="inlineStr">
         <is>
-          <t>eget metus eu erat semper rutrum. Fusce dolor quam, elementum</t>
+          <t>amet, consectetuer adipiscing elit. Etiam laoreet, libero et tristique pellentesque,</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>Lysandra Salas</t>
+          <t>Rafael Hanson</t>
         </is>
       </c>
       <c r="B72" s="0" t="inlineStr">
         <is>
-          <t>1-554-384-3169</t>
+          <t>(890) 923-1535</t>
         </is>
       </c>
       <c r="C72" s="0" t="inlineStr">
         <is>
-          <t>nec.ante@yahoo.org</t>
+          <t>mi.felis@outlook.couk</t>
         </is>
       </c>
       <c r="D72" s="0" t="inlineStr">
         <is>
-          <t>Illes Balears</t>
+          <t>Tyrol</t>
         </is>
       </c>
       <c r="E72" s="0" t="inlineStr">
         <is>
-          <t>Costa Rica</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="F72" s="0" t="inlineStr">
         <is>
-          <t>ullamcorper. Duis cursus, diam at pretium aliquet, metus urna convallis</t>
+          <t>nec, eleifend non, dapibus rutrum, justo. Praesent luctus. Curabitur egestas</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>Jin White</t>
+          <t>Ivan Golden</t>
         </is>
       </c>
       <c r="B73" s="0" t="inlineStr">
         <is>
-          <t>1-354-281-1488</t>
+          <t>1-771-782-8493</t>
         </is>
       </c>
       <c r="C73" s="0" t="inlineStr">
         <is>
-          <t>et.magnis.dis@aol.org</t>
+          <t>nisi.mauris@google.org</t>
         </is>
       </c>
       <c r="D73" s="0" t="inlineStr">
         <is>
-          <t>Queensland</t>
+          <t>Guanacaste</t>
         </is>
       </c>
       <c r="E73" s="0" t="inlineStr">
         <is>
-          <t>Mexico</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="F73" s="0" t="inlineStr">
         <is>
-          <t>euismod et, commodo at, libero. Morbi accumsan laoreet ipsum. Curabitur</t>
+          <t>molestie sodales. Mauris blandit enim consequat purus. Maecenas libero est,</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>Quynn Blevins</t>
+          <t>Michelle Barr</t>
         </is>
       </c>
       <c r="B74" s="0" t="inlineStr">
         <is>
-          <t>1-897-374-7724</t>
+          <t>1-235-912-5165</t>
         </is>
       </c>
       <c r="C74" s="0" t="inlineStr">
         <is>
-          <t>donec.egestas@hotmail.couk</t>
+          <t>arcu.sed@outlook.edu</t>
         </is>
       </c>
       <c r="D74" s="0" t="inlineStr">
         <is>
-          <t>Provence-Alpes-Côte d'Azur</t>
+          <t>Stockholms län</t>
         </is>
       </c>
       <c r="E74" s="0" t="inlineStr">
         <is>
-          <t>Australia</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F74" s="0" t="inlineStr">
         <is>
-          <t>Nulla aliquet. Proin velit. Sed malesuada augue ut lacus. Nulla</t>
+          <t>Quisque purus sapien, gravida non, sollicitudin a, malesuada id, erat.</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>Violet Boone</t>
+          <t>Lara Hunter</t>
         </is>
       </c>
       <c r="B75" s="0" t="inlineStr">
         <is>
-          <t>(317) 282-1687</t>
+          <t>1-688-663-9027</t>
         </is>
       </c>
       <c r="C75" s="0" t="inlineStr">
         <is>
-          <t>nunc.id@google.couk</t>
+          <t>ultrices.mauris.ipsum@hotmail.com</t>
         </is>
       </c>
       <c r="D75" s="0" t="inlineStr">
         <is>
-          <t>South Chungcheong</t>
+          <t>Dalarnas län</t>
         </is>
       </c>
       <c r="E75" s="0" t="inlineStr">
@@ -2477,445 +2477,445 @@
       </c>
       <c r="F75" s="0" t="inlineStr">
         <is>
-          <t>arcu. Aliquam ultrices iaculis odio. Nam interdum enim non nisi.</t>
+          <t>malesuada vel, convallis in, cursus et, eros. Proin ultrices. Duis</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>Carissa Chen</t>
+          <t>Palmer Stephens</t>
         </is>
       </c>
       <c r="B76" s="0" t="inlineStr">
         <is>
-          <t>1-153-774-0622</t>
+          <t>1-967-908-5115</t>
         </is>
       </c>
       <c r="C76" s="0" t="inlineStr">
         <is>
-          <t>integer.vitae.nibh@google.couk</t>
+          <t>fringilla.ornare.placerat@yahoo.net</t>
         </is>
       </c>
       <c r="D76" s="0" t="inlineStr">
         <is>
-          <t>Western Australia</t>
+          <t>Central Luzon</t>
         </is>
       </c>
       <c r="E76" s="0" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="F76" s="0" t="inlineStr">
         <is>
-          <t>ante bibendum ullamcorper. Duis cursus, diam at pretium aliquet, metus</t>
+          <t>aliquet diam. Sed diam lorem, auctor quis, tristique ac, eleifend</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>Samuel Mcmillan</t>
+          <t>Carissa Wall</t>
         </is>
       </c>
       <c r="B77" s="0" t="inlineStr">
         <is>
-          <t>(752) 666-5470</t>
+          <t>(255) 764-4428</t>
         </is>
       </c>
       <c r="C77" s="0" t="inlineStr">
         <is>
-          <t>mi.enim@aol.net</t>
+          <t>eget@yahoo.org</t>
         </is>
       </c>
       <c r="D77" s="0" t="inlineStr">
         <is>
-          <t>Rheinland-Pfalz</t>
+          <t>North Island</t>
         </is>
       </c>
       <c r="E77" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F77" s="0" t="inlineStr">
         <is>
-          <t>fermentum convallis ligula. Donec luctus aliquet odio. Etiam ligula tortor,</t>
+          <t>aliquet, sem ut cursus luctus, ipsum leo elementum sem, vitae</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>Hu Massey</t>
+          <t>Christopher Contreras</t>
         </is>
       </c>
       <c r="B78" s="0" t="inlineStr">
         <is>
-          <t>(412) 623-6779</t>
+          <t>1-274-592-2383</t>
         </is>
       </c>
       <c r="C78" s="0" t="inlineStr">
         <is>
-          <t>metus.vitae@outlook.couk</t>
+          <t>penatibus.et@outlook.org</t>
         </is>
       </c>
       <c r="D78" s="0" t="inlineStr">
         <is>
-          <t>Munster</t>
+          <t>Samsun</t>
         </is>
       </c>
       <c r="E78" s="0" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F78" s="0" t="inlineStr">
         <is>
-          <t>penatibus et magnis dis parturient montes, nascetur ridiculus mus. Proin</t>
+          <t>lacus, varius et, euismod et, commodo at, libero. Morbi accumsan</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>Declan Maxwell</t>
+          <t>Vernon Lindsay</t>
         </is>
       </c>
       <c r="B79" s="0" t="inlineStr">
         <is>
-          <t>1-384-897-3631</t>
+          <t>1-153-759-7637</t>
         </is>
       </c>
       <c r="C79" s="0" t="inlineStr">
         <is>
-          <t>consectetuer@aol.com</t>
+          <t>sed@outlook.org</t>
         </is>
       </c>
       <c r="D79" s="0" t="inlineStr">
         <is>
-          <t>Limpopo</t>
+          <t>Viken</t>
         </is>
       </c>
       <c r="E79" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F79" s="0" t="inlineStr">
         <is>
-          <t>pellentesque eget, dictum placerat, augue. Sed molestie. Sed id risus</t>
+          <t>cursus vestibulum. Mauris magna. Duis dignissim tempor arcu. Vestibulum ut</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>Ryder Ware</t>
+          <t>Ciaran Waters</t>
         </is>
       </c>
       <c r="B80" s="0" t="inlineStr">
         <is>
-          <t>1-412-364-7808</t>
+          <t>(814) 588-3742</t>
         </is>
       </c>
       <c r="C80" s="0" t="inlineStr">
         <is>
-          <t>vestibulum.accumsan.neque@google.edu</t>
+          <t>augue@aol.edu</t>
         </is>
       </c>
       <c r="D80" s="0" t="inlineStr">
         <is>
-          <t>Ulster</t>
+          <t>Arica y Parinacota</t>
         </is>
       </c>
       <c r="E80" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F80" s="0" t="inlineStr">
         <is>
-          <t>vulputate ullamcorper magna. Sed eu eros. Nam consequat dolor vitae</t>
+          <t>pharetra nibh. Aliquam ornare, libero at auctor ullamcorper, nisl arcu</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>Dahlia Horn</t>
+          <t>Benedict Vargas</t>
         </is>
       </c>
       <c r="B81" s="0" t="inlineStr">
         <is>
-          <t>1-513-714-7485</t>
+          <t>(227) 485-5949</t>
         </is>
       </c>
       <c r="C81" s="0" t="inlineStr">
         <is>
-          <t>ipsum.dolor@hotmail.org</t>
+          <t>magnis.dis@google.couk</t>
         </is>
       </c>
       <c r="D81" s="0" t="inlineStr">
         <is>
-          <t>Los Ríos</t>
+          <t>Hessen</t>
         </is>
       </c>
       <c r="E81" s="0" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="F81" s="0" t="inlineStr">
         <is>
-          <t>ipsum. Donec sollicitudin adipiscing ligula. Aenean gravida nunc sed pede.</t>
+          <t>mus. Donec dignissim magna a tortor. Nunc commodo auctor velit.</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>Orlando Donaldson</t>
+          <t>Shelly Browning</t>
         </is>
       </c>
       <c r="B82" s="0" t="inlineStr">
         <is>
-          <t>1-855-754-7647</t>
+          <t>(469) 556-4742</t>
         </is>
       </c>
       <c r="C82" s="0" t="inlineStr">
         <is>
-          <t>tellus.aenean@icloud.edu</t>
+          <t>elementum@protonmail.ca</t>
         </is>
       </c>
       <c r="D82" s="0" t="inlineStr">
         <is>
-          <t>Tasmania</t>
+          <t>Jönköpings län</t>
         </is>
       </c>
       <c r="E82" s="0" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F82" s="0" t="inlineStr">
         <is>
-          <t>elit elit fermentum risus, at fringilla purus mauris a nunc.</t>
+          <t>In scelerisque scelerisque dui. Suspendisse ac metus vitae velit egestas</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>Kylan Shelton</t>
+          <t>Branden Miles</t>
         </is>
       </c>
       <c r="B83" s="0" t="inlineStr">
         <is>
-          <t>(787) 788-3535</t>
+          <t>1-625-347-8946</t>
         </is>
       </c>
       <c r="C83" s="0" t="inlineStr">
         <is>
-          <t>dictum.augue@protonmail.edu</t>
+          <t>placerat.cras.dictum@outlook.couk</t>
         </is>
       </c>
       <c r="D83" s="0" t="inlineStr">
         <is>
-          <t>Antalya</t>
+          <t>Bà Rịa–Vũng Tàu</t>
         </is>
       </c>
       <c r="E83" s="0" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Singapore</t>
         </is>
       </c>
       <c r="F83" s="0" t="inlineStr">
         <is>
-          <t>ligula. Aenean gravida nunc sed pede. Cum sociis natoque penatibus</t>
+          <t>pulvinar arcu et pede. Nunc sed orci lobortis augue scelerisque</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>Shana Tate</t>
+          <t>Carla Vargas</t>
         </is>
       </c>
       <c r="B84" s="0" t="inlineStr">
         <is>
-          <t>1-483-363-3620</t>
+          <t>1-781-382-7173</t>
         </is>
       </c>
       <c r="C84" s="0" t="inlineStr">
         <is>
-          <t>suspendisse@icloud.net</t>
+          <t>non.lacinia@icloud.couk</t>
         </is>
       </c>
       <c r="D84" s="0" t="inlineStr">
         <is>
-          <t>North Region</t>
+          <t>Gaziantep</t>
         </is>
       </c>
       <c r="E84" s="0" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F84" s="0" t="inlineStr">
         <is>
-          <t>arcu. Nunc mauris. Morbi non sapien molestie orci tincidunt adipiscing.</t>
+          <t>turpis. Aliquam adipiscing lobortis risus. In mi pede, nonummy ut,</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>Jesse Colon</t>
+          <t>Juliet Colon</t>
         </is>
       </c>
       <c r="B85" s="0" t="inlineStr">
         <is>
-          <t>1-154-708-6487</t>
+          <t>(467) 337-3249</t>
         </is>
       </c>
       <c r="C85" s="0" t="inlineStr">
         <is>
-          <t>nec.diam.duis@outlook.org</t>
+          <t>cras.vulputate@outlook.edu</t>
         </is>
       </c>
       <c r="D85" s="0" t="inlineStr">
         <is>
-          <t>Limburg</t>
+          <t>Tyrol</t>
         </is>
       </c>
       <c r="E85" s="0" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="F85" s="0" t="inlineStr">
         <is>
-          <t>cursus. Integer mollis. Integer tincidunt aliquam arcu. Aliquam ultrices iaculis</t>
+          <t>netus et malesuada fames ac turpis egestas. Fusce aliquet magna</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>Kyla Gay</t>
+          <t>Alexis Coffey</t>
         </is>
       </c>
       <c r="B86" s="0" t="inlineStr">
         <is>
-          <t>1-814-435-4161</t>
+          <t>1-328-218-8848</t>
         </is>
       </c>
       <c r="C86" s="0" t="inlineStr">
         <is>
-          <t>donec.nibh@icloud.ca</t>
+          <t>metus.vitae@hotmail.org</t>
         </is>
       </c>
       <c r="D86" s="0" t="inlineStr">
         <is>
-          <t>Nizhny Novgorod Oblast</t>
+          <t>Veracruz</t>
         </is>
       </c>
       <c r="E86" s="0" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Australia</t>
         </is>
       </c>
       <c r="F86" s="0" t="inlineStr">
         <is>
-          <t>ac turpis egestas. Aliquam fringilla cursus purus. Nullam scelerisque neque</t>
+          <t>scelerisque scelerisque dui. Suspendisse ac metus vitae velit egestas lacinia.</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>Cullen Singleton</t>
+          <t>Igor Acosta</t>
         </is>
       </c>
       <c r="B87" s="0" t="inlineStr">
         <is>
-          <t>(324) 874-6756</t>
+          <t>(604) 427-5546</t>
         </is>
       </c>
       <c r="C87" s="0" t="inlineStr">
         <is>
-          <t>leo.in@hotmail.couk</t>
+          <t>venenatis.vel@google.net</t>
         </is>
       </c>
       <c r="D87" s="0" t="inlineStr">
         <is>
-          <t>Arica y Parinacota</t>
+          <t>Istanbul</t>
         </is>
       </c>
       <c r="E87" s="0" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Colombia</t>
         </is>
       </c>
       <c r="F87" s="0" t="inlineStr">
         <is>
-          <t>sit amet ante. Vivamus non lorem vitae odio sagittis semper.</t>
+          <t>vulputate, posuere vulputate, lacus. Cras interdum. Nunc sollicitudin commodo ipsum.</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>Zenia Cameron</t>
+          <t>Baxter Wilkinson</t>
         </is>
       </c>
       <c r="B88" s="0" t="inlineStr">
         <is>
-          <t>(982) 353-1632</t>
+          <t>(858) 160-6944</t>
         </is>
       </c>
       <c r="C88" s="0" t="inlineStr">
         <is>
-          <t>facilisis@aol.com</t>
+          <t>aliquet@yahoo.org</t>
         </is>
       </c>
       <c r="D88" s="0" t="inlineStr">
         <is>
-          <t>Cajamarca</t>
+          <t>Limón</t>
         </is>
       </c>
       <c r="E88" s="0" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>South Korea</t>
         </is>
       </c>
       <c r="F88" s="0" t="inlineStr">
         <is>
-          <t>interdum ligula eu enim. Etiam imperdiet dictum magna. Ut tincidunt</t>
+          <t>eleifend. Cras sed leo. Cras vehicula aliquet libero. Integer in</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>Amanda Gay</t>
+          <t>Darryl Burnett</t>
         </is>
       </c>
       <c r="B89" s="0" t="inlineStr">
         <is>
-          <t>1-444-795-0313</t>
+          <t>(665) 929-8195</t>
         </is>
       </c>
       <c r="C89" s="0" t="inlineStr">
         <is>
-          <t>sit.amet@outlook.couk</t>
+          <t>morbi.tristique@google.com</t>
         </is>
       </c>
       <c r="D89" s="0" t="inlineStr">
         <is>
-          <t>Brandenburg</t>
+          <t>Aberdeenshire</t>
         </is>
       </c>
       <c r="E89" s="0" t="inlineStr">
@@ -2925,391 +2925,391 @@
       </c>
       <c r="F89" s="0" t="inlineStr">
         <is>
-          <t>enim consequat purus. Maecenas libero est, congue a, aliquet vel,</t>
+          <t>magna. Suspendisse tristique neque venenatis lacus. Etiam bibendum fermentum metus.</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>Cynthia Savage</t>
+          <t>Joseph Robinson</t>
         </is>
       </c>
       <c r="B90" s="0" t="inlineStr">
         <is>
-          <t>(168) 385-4454</t>
+          <t>(377) 749-1131</t>
         </is>
       </c>
       <c r="C90" s="0" t="inlineStr">
         <is>
-          <t>diam.nunc.ullamcorper@yahoo.couk</t>
+          <t>fringilla@protonmail.org</t>
         </is>
       </c>
       <c r="D90" s="0" t="inlineStr">
         <is>
-          <t>Zamboanga Peninsula</t>
+          <t>Querétaro</t>
         </is>
       </c>
       <c r="E90" s="0" t="inlineStr">
         <is>
-          <t>New Zealand</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="F90" s="0" t="inlineStr">
         <is>
-          <t>dictum magna. Ut tincidunt orci quis lectus. Nullam suscipit, est</t>
+          <t>Sed eget lacus. Mauris non dui nec urna suscipit nonummy.</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>Nina Sellers</t>
+          <t>Martin Goodman</t>
         </is>
       </c>
       <c r="B91" s="0" t="inlineStr">
         <is>
-          <t>(380) 460-4786</t>
+          <t>(773) 603-1563</t>
         </is>
       </c>
       <c r="C91" s="0" t="inlineStr">
         <is>
-          <t>sed.pede@hotmail.org</t>
+          <t>nec.euismod@yahoo.ca</t>
         </is>
       </c>
       <c r="D91" s="0" t="inlineStr">
         <is>
-          <t>San Luis Potosí</t>
+          <t>Istanbul</t>
         </is>
       </c>
       <c r="E91" s="0" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="F91" s="0" t="inlineStr">
         <is>
-          <t>urna justo faucibus lectus, a sollicitudin orci sem eget massa.</t>
+          <t>nunc nulla vulputate dui, nec tempus mauris erat eget ipsum.</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>Levi Burch</t>
+          <t>TaShya Bowen</t>
         </is>
       </c>
       <c r="B92" s="0" t="inlineStr">
         <is>
-          <t>(578) 988-4883</t>
+          <t>(469) 645-2545</t>
         </is>
       </c>
       <c r="C92" s="0" t="inlineStr">
         <is>
-          <t>eu@hotmail.net</t>
+          <t>cum.sociis@protonmail.couk</t>
         </is>
       </c>
       <c r="D92" s="0" t="inlineStr">
         <is>
-          <t>Limpopo</t>
+          <t>Guanacaste</t>
         </is>
       </c>
       <c r="E92" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Mexico</t>
         </is>
       </c>
       <c r="F92" s="0" t="inlineStr">
         <is>
-          <t>ultrices. Vivamus rhoncus. Donec est. Nunc ullamcorper, velit in aliquet</t>
+          <t>nascetur ridiculus mus. Donec dignissim magna a tortor. Nunc commodo</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>Charles Hess</t>
+          <t>Imelda Rivers</t>
         </is>
       </c>
       <c r="B93" s="0" t="inlineStr">
         <is>
-          <t>1-258-286-7816</t>
+          <t>(468) 557-0776</t>
         </is>
       </c>
       <c r="C93" s="0" t="inlineStr">
         <is>
-          <t>risus.in.mi@outlook.com</t>
+          <t>eu.enim@aol.couk</t>
         </is>
       </c>
       <c r="D93" s="0" t="inlineStr">
         <is>
-          <t>Madrid</t>
+          <t>Sikkim</t>
         </is>
       </c>
       <c r="E93" s="0" t="inlineStr">
         <is>
-          <t>Vietnam</t>
+          <t>China</t>
         </is>
       </c>
       <c r="F93" s="0" t="inlineStr">
         <is>
-          <t>molestie tellus. Aenean egestas hendrerit neque. In ornare sagittis felis.</t>
+          <t>ante. Nunc mauris sapien, cursus in, hendrerit consectetuer, cursus et,</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>Lydia Flowers</t>
+          <t>Connor Calderon</t>
         </is>
       </c>
       <c r="B94" s="0" t="inlineStr">
         <is>
-          <t>1-277-377-5676</t>
+          <t>(554) 832-1532</t>
         </is>
       </c>
       <c r="C94" s="0" t="inlineStr">
         <is>
-          <t>quis@yahoo.ca</t>
+          <t>penatibus@outlook.com</t>
         </is>
       </c>
       <c r="D94" s="0" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>Franche-Comté</t>
         </is>
       </c>
       <c r="E94" s="0" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F94" s="0" t="inlineStr">
         <is>
-          <t>placerat, augue. Sed molestie. Sed id risus quis diam luctus</t>
+          <t>varius. Nam porttitor scelerisque neque. Nullam nisl. Maecenas malesuada fringilla</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>Illana Nunez</t>
+          <t>Harriet Beard</t>
         </is>
       </c>
       <c r="B95" s="0" t="inlineStr">
         <is>
-          <t>(769) 475-7664</t>
+          <t>(462) 786-4245</t>
         </is>
       </c>
       <c r="C95" s="0" t="inlineStr">
         <is>
-          <t>sem.eget@protonmail.com</t>
+          <t>nisi.nibh@google.couk</t>
         </is>
       </c>
       <c r="D95" s="0" t="inlineStr">
         <is>
-          <t>Junín</t>
+          <t>Murcia</t>
         </is>
       </c>
       <c r="E95" s="0" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Brazil</t>
         </is>
       </c>
       <c r="F95" s="0" t="inlineStr">
         <is>
-          <t>lacus. Ut nec urna et arcu imperdiet ullamcorper. Duis at</t>
+          <t>ultricies adipiscing, enim mi tempor lorem, eget mollis lectus pede</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>Ishmael Burgess</t>
+          <t>Ishmael Odom</t>
         </is>
       </c>
       <c r="B96" s="0" t="inlineStr">
         <is>
-          <t>1-473-866-4498</t>
+          <t>(849) 972-1834</t>
         </is>
       </c>
       <c r="C96" s="0" t="inlineStr">
         <is>
-          <t>ridiculus.mus@hotmail.net</t>
+          <t>laoreet.lectus@yahoo.com</t>
         </is>
       </c>
       <c r="D96" s="0" t="inlineStr">
         <is>
-          <t>Aragón</t>
+          <t>Haryana</t>
         </is>
       </c>
       <c r="E96" s="0" t="inlineStr">
         <is>
-          <t>Peru</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="F96" s="0" t="inlineStr">
         <is>
-          <t>nulla. Integer urna. Vivamus molestie dapibus ligula. Aliquam erat volutpat.</t>
+          <t>Nullam feugiat placerat velit. Quisque varius. Nam porttitor scelerisque neque.</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>Asher Cobb</t>
+          <t>Virginia Ayers</t>
         </is>
       </c>
       <c r="B97" s="0" t="inlineStr">
         <is>
-          <t>(913) 361-6683</t>
+          <t>(605) 308-2148</t>
         </is>
       </c>
       <c r="C97" s="0" t="inlineStr">
         <is>
-          <t>eros.nam@icloud.ca</t>
+          <t>a.purus@protonmail.net</t>
         </is>
       </c>
       <c r="D97" s="0" t="inlineStr">
         <is>
-          <t>Omsk Oblast</t>
+          <t>Xīběi</t>
         </is>
       </c>
       <c r="E97" s="0" t="inlineStr">
         <is>
-          <t>South Korea</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="F97" s="0" t="inlineStr">
         <is>
-          <t>rutrum. Fusce dolor quam, elementum at, egestas a, scelerisque sed,</t>
+          <t>iaculis odio. Nam interdum enim non nisi. Aenean eget metus.</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>Iris Diaz</t>
+          <t>Brendan Cole</t>
         </is>
       </c>
       <c r="B98" s="0" t="inlineStr">
         <is>
-          <t>1-647-887-7863</t>
+          <t>(753) 418-7279</t>
         </is>
       </c>
       <c r="C98" s="0" t="inlineStr">
         <is>
-          <t>elit@hotmail.ca</t>
+          <t>cras.sed@icloud.ca</t>
         </is>
       </c>
       <c r="D98" s="0" t="inlineStr">
         <is>
-          <t>Connacht</t>
+          <t>Podlaskie</t>
         </is>
       </c>
       <c r="E98" s="0" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="F98" s="0" t="inlineStr">
         <is>
-          <t>mauris ut mi. Duis risus odio, auctor vitae, aliquet nec,</t>
+          <t>est arcu ac orci. Ut semper pretium neque. Morbi quis</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>Calvin Barry</t>
+          <t>Nichole Wynn</t>
         </is>
       </c>
       <c r="B99" s="0" t="inlineStr">
         <is>
-          <t>1-271-938-4740</t>
+          <t>(116) 962-6750</t>
         </is>
       </c>
       <c r="C99" s="0" t="inlineStr">
         <is>
-          <t>a@outlook.ca</t>
+          <t>cursus@hotmail.edu</t>
         </is>
       </c>
       <c r="D99" s="0" t="inlineStr">
         <is>
-          <t>West Nusa Tenggara</t>
+          <t>Bayern</t>
         </is>
       </c>
       <c r="E99" s="0" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="F99" s="0" t="inlineStr">
         <is>
-          <t>elit fermentum risus, at fringilla purus mauris a nunc. In</t>
+          <t>lorem tristique aliquet. Phasellus fermentum convallis ligula. Donec luctus aliquet</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>Allegra Lowery</t>
+          <t>Beverly Mays</t>
         </is>
       </c>
       <c r="B100" s="0" t="inlineStr">
         <is>
-          <t>(322) 390-8158</t>
+          <t>(770) 803-4352</t>
         </is>
       </c>
       <c r="C100" s="0" t="inlineStr">
         <is>
-          <t>inceptos@outlook.edu</t>
+          <t>nisi.nibh@icloud.edu</t>
         </is>
       </c>
       <c r="D100" s="0" t="inlineStr">
         <is>
-          <t>Eastern Cape</t>
+          <t>Sląskie</t>
         </is>
       </c>
       <c r="E100" s="0" t="inlineStr">
         <is>
-          <t>Colombia</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="F100" s="0" t="inlineStr">
         <is>
-          <t>Sed et libero. Proin mi. Aliquam gravida mauris ut mi.</t>
+          <t>massa. Integer vitae nibh. Donec est mauris, rhoncus id, mollis</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>Yvonne Buckley</t>
+          <t>Kalia Marquez</t>
         </is>
       </c>
       <c r="B101" s="0" t="inlineStr">
         <is>
-          <t>1-762-730-6322</t>
+          <t>1-687-741-4375</t>
         </is>
       </c>
       <c r="C101" s="0" t="inlineStr">
         <is>
-          <t>odio.a@protonmail.ca</t>
+          <t>ridiculus.mus.aenean@aol.couk</t>
         </is>
       </c>
       <c r="D101" s="0" t="inlineStr">
         <is>
-          <t>Friesland</t>
+          <t>Irkutsk Oblast</t>
         </is>
       </c>
       <c r="E101" s="0" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>Russian Federation</t>
         </is>
       </c>
       <c r="F101" s="0" t="inlineStr">
         <is>
-          <t>ante ipsum primis in faucibus orci luctus et ultrices posuere</t>
+          <t>amet diam eu dolor egestas rhoncus. Proin nisl sem, consequat</t>
         </is>
       </c>
     </row>

</xml_diff>